<commit_message>
small changes tp lab4 info
</commit_message>
<xml_diff>
--- a/Informatics/lab4.xlsx
+++ b/Informatics/lab4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\ITMO-Labs\Informatics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA3266A-8F9F-409C-96BA-A7EF7014FC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1553B4D3-CCB8-4AEB-98F0-2DA3E262472F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B976E2FC-2D12-4AD0-A34B-F86A3C86067F}"/>
   </bookViews>
@@ -321,34 +321,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -409,6 +403,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-DBC3-48CB-81E7-DB38DCABED0C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -424,6 +423,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-DBC3-48CB-81E7-DB38DCABED0C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -439,6 +443,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-DBC3-48CB-81E7-DB38DCABED0C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -454,6 +463,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-DBC3-48CB-81E7-DB38DCABED0C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -469,6 +483,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-DBC3-48CB-81E7-DB38DCABED0C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -484,6 +503,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-DBC3-48CB-81E7-DB38DCABED0C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -501,6 +525,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-DBC3-48CB-81E7-DB38DCABED0C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -518,6 +547,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-DBC3-48CB-81E7-DB38DCABED0C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -535,6 +569,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-DBC3-48CB-81E7-DB38DCABED0C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -552,6 +591,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-DBC3-48CB-81E7-DB38DCABED0C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -569,6 +613,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-DBC3-48CB-81E7-DB38DCABED0C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -586,6 +635,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-DBC3-48CB-81E7-DB38DCABED0C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -1632,7 +1686,7 @@
   <dimension ref="A1:AK58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE12" sqref="AE12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1664,27 +1718,27 @@
       <c r="C2">
         <v>25449</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2126,7 +2180,7 @@
         <v>25</v>
       </c>
       <c r="C10">
-        <f>-1 * C4</f>
+        <f>-C4</f>
         <v>-2404</v>
       </c>
       <c r="E10" t="s">
@@ -2217,7 +2271,7 @@
         <v>26</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C15" si="0">-1 * C5</f>
+        <f>-C5</f>
         <v>-25449</v>
       </c>
       <c r="E11" t="s">
@@ -2308,7 +2362,7 @@
         <v>27</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C12:C15" si="0">-C6</f>
         <v>-27853</v>
       </c>
       <c r="E12" t="s">
@@ -2665,10 +2719,10 @@
       </c>
     </row>
     <row r="18" spans="3:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="9">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F18" t="s">
@@ -2750,7 +2804,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AC18" s="4" t="s">
+      <c r="AC18" s="6" t="s">
         <v>57</v>
       </c>
       <c r="AD18" t="s">
@@ -2760,17 +2814,17 @@
         <f>C4</f>
         <v>2404</v>
       </c>
-      <c r="AG18" s="6" t="s">
+      <c r="AG18" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="AH18" s="6"/>
-      <c r="AI18" s="6"/>
-      <c r="AJ18" s="6"/>
-      <c r="AK18" s="6"/>
+      <c r="AH18" s="7"/>
+      <c r="AI18" s="7"/>
+      <c r="AJ18" s="7"/>
+      <c r="AK18" s="7"/>
     </row>
     <row r="19" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C19" s="9"/>
-      <c r="E19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="E19" s="6"/>
       <c r="F19" t="s">
         <v>32</v>
       </c>
@@ -2850,7 +2904,7 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="AC19" s="4"/>
+      <c r="AC19" s="6"/>
       <c r="AD19" t="s">
         <v>4</v>
       </c>
@@ -2858,87 +2912,87 @@
         <f>C5</f>
         <v>25449</v>
       </c>
-      <c r="AG19" s="6"/>
-      <c r="AH19" s="6"/>
-      <c r="AI19" s="6"/>
-      <c r="AJ19" s="6"/>
-      <c r="AK19" s="6"/>
+      <c r="AG19" s="7"/>
+      <c r="AH19" s="7"/>
+      <c r="AI19" s="7"/>
+      <c r="AJ19" s="7"/>
+      <c r="AK19" s="7"/>
     </row>
     <row r="20" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C20" s="9"/>
-      <c r="G20" s="7">
+      <c r="C20" s="5"/>
+      <c r="G20" s="3">
         <f t="shared" ref="G20" si="5">IF(SUM(G18:G19) + IF(OR(SUM(H18:H19)=2,AND(SUM(H18:H19)=1,H20=0)), 1, 0) &lt; 2, SUM(G18:G19) + IF(OR(SUM(H18:H19)=2,AND(SUM(H18:H19)=1,H20=0)), 1, 0), SUM(G18:G19) + IF(OR(SUM(H18:H19)=2,AND(SUM(H18:H19)=1,H20=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="3">
         <f t="shared" ref="H20" si="6">IF(SUM(H18:H19) + IF(OR(SUM(I18:I19)=2,AND(SUM(I18:I19)=1,I20=0)), 1, 0) &lt; 2, SUM(H18:H19) + IF(OR(SUM(I18:I19)=2,AND(SUM(I18:I19)=1,I20=0)), 1, 0), SUM(H18:H19) + IF(OR(SUM(I18:I19)=2,AND(SUM(I18:I19)=1,I20=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="3">
         <f>IF(SUM(I18:I19) + IF(OR(SUM(J18:J19)=2,AND(SUM(J18:J19)=1,J20=0)), 1, 0) &lt; 2, SUM(I18:I19) + IF(OR(SUM(J18:J19)=2,AND(SUM(J18:J19)=1,J20=0)), 1, 0), SUM(I18:I19) + IF(OR(SUM(J18:J19)=2,AND(SUM(J18:J19)=1,J20=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="3">
         <f>IF(SUM(J18:J19) + IF(OR(SUM(L18:L19)=2,AND(SUM(L18:L19)=1,L20=0)), 1, 0) &lt; 2, SUM(J18:J19) + IF(OR(SUM(L18:L19)=2,AND(SUM(L18:L19)=1,L20=0)), 1, 0), SUM(J18:J19) + IF(OR(SUM(L18:L19)=2,AND(SUM(L18:L19)=1,L20=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="7" t="str">
+      <c r="K20" s="3" t="str">
         <f t="shared" si="4"/>
         <v>.</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="3">
         <f t="shared" ref="L20" si="7">IF(SUM(L18:L19) + IF(OR(SUM(M18:M19)=2,AND(SUM(M18:M19)=1,M20=0)), 1, 0) &lt; 2, SUM(L18:L19) + IF(OR(SUM(M18:M19)=2,AND(SUM(M18:M19)=1,M20=0)), 1, 0), SUM(L18:L19) + IF(OR(SUM(M18:M19)=2,AND(SUM(M18:M19)=1,M20=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M20" s="3">
         <f t="shared" ref="M20" si="8">IF(SUM(M18:M19) + IF(OR(SUM(N18:N19)=2,AND(SUM(N18:N19)=1,N20=0)), 1, 0) &lt; 2, SUM(M18:M19) + IF(OR(SUM(N18:N19)=2,AND(SUM(N18:N19)=1,N20=0)), 1, 0), SUM(M18:M19) + IF(OR(SUM(N18:N19)=2,AND(SUM(N18:N19)=1,N20=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N20" s="3">
         <f>IF(SUM(N18:N19) + IF(OR(SUM(O18:O19)=2,AND(SUM(O18:O19)=1,O20=0)), 1, 0) &lt; 2, SUM(N18:N19) + IF(OR(SUM(O18:O19)=2,AND(SUM(O18:O19)=1,O20=0)), 1, 0), SUM(N18:N19) + IF(OR(SUM(O18:O19)=2,AND(SUM(O18:O19)=1,O20=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="7">
+      <c r="O20" s="3">
         <f>IF(SUM(O18:O19) + IF(OR(SUM(Q18:Q19)=2,AND(SUM(Q18:Q19)=1,Q20=0)), 1, 0) &lt; 2, SUM(O18:O19) + IF(OR(SUM(Q18:Q19)=2,AND(SUM(Q18:Q19)=1,Q20=0)), 1, 0), SUM(O18:O19) + IF(OR(SUM(Q18:Q19)=2,AND(SUM(Q18:Q19)=1,Q20=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="P20" s="7" t="str">
+      <c r="P20" s="3" t="str">
         <f t="shared" si="4"/>
         <v>.</v>
       </c>
-      <c r="Q20" s="7">
+      <c r="Q20" s="3">
         <f t="shared" ref="Q20" si="9">IF(SUM(Q18:Q19) + IF(OR(SUM(R18:R19)=2,AND(SUM(R18:R19)=1,R20=0)), 1, 0) &lt; 2, SUM(Q18:Q19) + IF(OR(SUM(R18:R19)=2,AND(SUM(R18:R19)=1,R20=0)), 1, 0), SUM(Q18:Q19) + IF(OR(SUM(R18:R19)=2,AND(SUM(R18:R19)=1,R20=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="R20" s="7">
+      <c r="R20" s="3">
         <f t="shared" ref="R20" si="10">IF(SUM(R18:R19) + IF(OR(SUM(S18:S19)=2,AND(SUM(S18:S19)=1,S20=0)), 1, 0) &lt; 2, SUM(R18:R19) + IF(OR(SUM(S18:S19)=2,AND(SUM(S18:S19)=1,S20=0)), 1, 0), SUM(R18:R19) + IF(OR(SUM(S18:S19)=2,AND(SUM(S18:S19)=1,S20=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="S20" s="7">
+      <c r="S20" s="3">
         <f>IF(SUM(S18:S19) + IF(OR(SUM(T18:T19)=2,AND(SUM(T18:T19)=1,T20=0)), 1, 0) &lt; 2, SUM(S18:S19) + IF(OR(SUM(T18:T19)=2,AND(SUM(T18:T19)=1,T20=0)), 1, 0), SUM(S18:S19) + IF(OR(SUM(T18:T19)=2,AND(SUM(T18:T19)=1,T20=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="T20" s="7">
+      <c r="T20" s="3">
         <f>IF(SUM(T18:T19) + IF(OR(SUM(V18:V19)=2,AND(SUM(V18:V19)=1,V20=0)), 1, 0) &lt; 2, SUM(T18:T19) + IF(OR(SUM(V18:V19)=2,AND(SUM(V18:V19)=1,V20=0)), 1, 0), SUM(T18:T19) + IF(OR(SUM(V18:V19)=2,AND(SUM(V18:V19)=1,V20=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="U20" s="7" t="str">
+      <c r="U20" s="3" t="str">
         <f t="shared" si="4"/>
         <v>.</v>
       </c>
-      <c r="V20" s="7">
+      <c r="V20" s="3">
         <f t="shared" ref="V20:W20" si="11">IF(SUM(V18:V19) + IF(OR(SUM(W18:W19)=2,AND(SUM(W18:W19)=1,W20=0)), 1, 0) &lt; 2, SUM(V18:V19) + IF(OR(SUM(W18:W19)=2,AND(SUM(W18:W19)=1,W20=0)), 1, 0), SUM(V18:V19) + IF(OR(SUM(W18:W19)=2,AND(SUM(W18:W19)=1,W20=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="W20" s="7">
+      <c r="W20" s="3">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="X20" s="7">
+      <c r="X20" s="3">
         <f>IF(SUM(X18:X19) + IF(OR(SUM(Y18:Y19)=2,AND(SUM(Y18:Y19)=1,Y20=0)), 1, 0) &lt; 2, SUM(X18:X19) + IF(OR(SUM(Y18:Y19)=2,AND(SUM(Y18:Y19)=1,Y20=0)), 1, 0), SUM(X18:X19) + IF(OR(SUM(Y18:Y19)=2,AND(SUM(Y18:Y19)=1,Y20=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="Y20" s="7">
+      <c r="Y20" s="3">
         <f>2 - (Y18 + Y19)</f>
         <v>1</v>
       </c>
@@ -2952,22 +3006,22 @@
         <f>AE18 + AE19</f>
         <v>27853</v>
       </c>
-      <c r="AG20" s="6"/>
-      <c r="AH20" s="6"/>
-      <c r="AI20" s="6"/>
-      <c r="AJ20" s="6"/>
-      <c r="AK20" s="6"/>
+      <c r="AG20" s="7"/>
+      <c r="AH20" s="7"/>
+      <c r="AI20" s="7"/>
+      <c r="AJ20" s="7"/>
+      <c r="AK20" s="7"/>
     </row>
     <row r="21" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C21" s="9"/>
-      <c r="AG21" s="6"/>
-      <c r="AH21" s="6"/>
-      <c r="AI21" s="6"/>
-      <c r="AJ21" s="6"/>
-      <c r="AK21" s="6"/>
+      <c r="C21" s="5"/>
+      <c r="AG21" s="7"/>
+      <c r="AH21" s="7"/>
+      <c r="AI21" s="7"/>
+      <c r="AJ21" s="7"/>
+      <c r="AK21" s="7"/>
     </row>
     <row r="22" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C22" s="9"/>
+      <c r="C22" s="5"/>
       <c r="F22" t="s">
         <v>59</v>
       </c>
@@ -2975,38 +3029,38 @@
         <f>IF(OR(SUM(G18:G19)=2,AND(SUM(G18:G19)=1,G20=0)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
       <c r="L22">
         <f>IF(ISEVEN(SUM(Q20:Y20)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="N22" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
       <c r="Q22">
         <f>IF(OR(SUM(V18:V19)=2,AND(SUM(V18:V19)=1,V20=0)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="S22" s="5" t="s">
+      <c r="S22" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
       <c r="V22">
         <f>IF(SUM(G20:Y20)=0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="X22" s="5" t="s">
+      <c r="X22" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="Y22" s="5"/>
-      <c r="Z22" s="5"/>
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="8"/>
       <c r="AA22">
         <f>G20</f>
         <v>0</v>
@@ -3018,99 +3072,99 @@
         <f>IF(OR(SUM(G18:G19)=2,AND(SUM(G18:G19)=1,G20=0)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="AG22" s="6"/>
-      <c r="AH22" s="6"/>
-      <c r="AI22" s="6"/>
-      <c r="AJ22" s="6"/>
-      <c r="AK22" s="6"/>
+      <c r="AG22" s="7"/>
+      <c r="AH22" s="7"/>
+      <c r="AI22" s="7"/>
+      <c r="AJ22" s="7"/>
+      <c r="AK22" s="7"/>
     </row>
     <row r="24" spans="3:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="9">
+      <c r="C24" s="5">
         <v>2</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F24" t="s">
         <v>32</v>
       </c>
       <c r="G24">
-        <f>G5</f>
+        <f t="shared" ref="G24:Y24" si="12">G5</f>
         <v>0</v>
       </c>
       <c r="H24">
-        <f>H5</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="I24">
-        <f>I5</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="J24">
-        <f>J5</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K24" t="str">
-        <f>K5</f>
+        <f t="shared" si="12"/>
         <v>.</v>
       </c>
       <c r="L24">
-        <f>L5</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M24">
-        <f>M5</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N24">
-        <f>N5</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="O24">
-        <f>O5</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="P24" t="str">
-        <f>P5</f>
+        <f t="shared" si="12"/>
         <v>.</v>
       </c>
       <c r="Q24">
-        <f>Q5</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="R24">
-        <f>R5</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="S24">
-        <f>S5</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="T24">
-        <f>T5</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="U24" t="str">
-        <f>U5</f>
+        <f t="shared" si="12"/>
         <v>.</v>
       </c>
       <c r="V24">
-        <f>V5</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="W24">
-        <f>W5</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X24">
-        <f>X5</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Y24">
-        <f>Y5</f>
-        <v>1</v>
-      </c>
-      <c r="AC24" s="4" t="s">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AC24" s="6" t="s">
         <v>57</v>
       </c>
       <c r="AD24" t="s">
@@ -3120,97 +3174,97 @@
         <f>C5</f>
         <v>25449</v>
       </c>
-      <c r="AG24" s="6" t="s">
+      <c r="AG24" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AH24" s="6"/>
-      <c r="AI24" s="6"/>
-      <c r="AJ24" s="6"/>
-      <c r="AK24" s="6"/>
+      <c r="AH24" s="7"/>
+      <c r="AI24" s="7"/>
+      <c r="AJ24" s="7"/>
+      <c r="AK24" s="7"/>
     </row>
     <row r="25" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C25" s="9"/>
-      <c r="E25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="E25" s="6"/>
       <c r="F25" t="s">
         <v>33</v>
       </c>
       <c r="G25">
-        <f>G6</f>
+        <f t="shared" ref="G25:Y25" si="13">G6</f>
         <v>0</v>
       </c>
       <c r="H25">
-        <f>H6</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="I25">
-        <f>I6</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J25">
-        <f>J6</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K25" t="str">
-        <f>K6</f>
+        <f t="shared" si="13"/>
         <v>.</v>
       </c>
       <c r="L25">
-        <f>L6</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M25">
-        <f>M6</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="N25">
-        <f>N6</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="O25">
-        <f>O6</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P25" t="str">
-        <f>P6</f>
+        <f t="shared" si="13"/>
         <v>.</v>
       </c>
       <c r="Q25">
-        <f>Q6</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="R25">
-        <f>R6</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="S25">
-        <f>S6</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T25">
-        <f>T6</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U25" t="str">
-        <f>U6</f>
+        <f t="shared" si="13"/>
         <v>.</v>
       </c>
       <c r="V25">
-        <f>V6</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="W25">
-        <f>W6</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="X25">
-        <f>X6</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Y25">
-        <f>Y6</f>
-        <v>1</v>
-      </c>
-      <c r="AC25" s="4"/>
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AC25" s="6"/>
       <c r="AD25" t="s">
         <v>5</v>
       </c>
@@ -3218,87 +3272,87 @@
         <f>C6</f>
         <v>27853</v>
       </c>
-      <c r="AG25" s="6"/>
-      <c r="AH25" s="6"/>
-      <c r="AI25" s="6"/>
-      <c r="AJ25" s="6"/>
-      <c r="AK25" s="6"/>
+      <c r="AG25" s="7"/>
+      <c r="AH25" s="7"/>
+      <c r="AI25" s="7"/>
+      <c r="AJ25" s="7"/>
+      <c r="AK25" s="7"/>
     </row>
     <row r="26" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C26" s="9"/>
-      <c r="G26" s="7">
-        <f t="shared" ref="G26" si="12">IF(SUM(G24:G25) + IF(OR(SUM(H24:H25)=2,AND(SUM(H24:H25)=1,H26=0)), 1, 0) &lt; 2, SUM(G24:G25) + IF(OR(SUM(H24:H25)=2,AND(SUM(H24:H25)=1,H26=0)), 1, 0), SUM(G24:G25) + IF(OR(SUM(H24:H25)=2,AND(SUM(H24:H25)=1,H26=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="H26" s="7">
-        <f t="shared" ref="H26" si="13">IF(SUM(H24:H25) + IF(OR(SUM(I24:I25)=2,AND(SUM(I24:I25)=1,I26=0)), 1, 0) &lt; 2, SUM(H24:H25) + IF(OR(SUM(I24:I25)=2,AND(SUM(I24:I25)=1,I26=0)), 1, 0), SUM(H24:H25) + IF(OR(SUM(I24:I25)=2,AND(SUM(I24:I25)=1,I26=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="I26" s="7">
+      <c r="C26" s="5"/>
+      <c r="G26" s="3">
+        <f t="shared" ref="G26" si="14">IF(SUM(G24:G25) + IF(OR(SUM(H24:H25)=2,AND(SUM(H24:H25)=1,H26=0)), 1, 0) &lt; 2, SUM(G24:G25) + IF(OR(SUM(H24:H25)=2,AND(SUM(H24:H25)=1,H26=0)), 1, 0), SUM(G24:G25) + IF(OR(SUM(H24:H25)=2,AND(SUM(H24:H25)=1,H26=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="H26" s="3">
+        <f t="shared" ref="H26" si="15">IF(SUM(H24:H25) + IF(OR(SUM(I24:I25)=2,AND(SUM(I24:I25)=1,I26=0)), 1, 0) &lt; 2, SUM(H24:H25) + IF(OR(SUM(I24:I25)=2,AND(SUM(I24:I25)=1,I26=0)), 1, 0), SUM(H24:H25) + IF(OR(SUM(I24:I25)=2,AND(SUM(I24:I25)=1,I26=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="I26" s="3">
         <f>IF(SUM(I24:I25) + IF(OR(SUM(J24:J25)=2,AND(SUM(J24:J25)=1,J26=0)), 1, 0) &lt; 2, SUM(I24:I25) + IF(OR(SUM(J24:J25)=2,AND(SUM(J24:J25)=1,J26=0)), 1, 0), SUM(I24:I25) + IF(OR(SUM(J24:J25)=2,AND(SUM(J24:J25)=1,J26=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="J26" s="7">
+      <c r="J26" s="3">
         <f>IF(SUM(J24:J25) + IF(OR(SUM(L24:L25)=2,AND(SUM(L24:L25)=1,L26=0)), 1, 0) &lt; 2, SUM(J24:J25) + IF(OR(SUM(L24:L25)=2,AND(SUM(L24:L25)=1,L26=0)), 1, 0), SUM(J24:J25) + IF(OR(SUM(L24:L25)=2,AND(SUM(L24:L25)=1,L26=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="K26" s="7" t="str">
-        <f t="shared" ref="K26:Y26" si="14">K12</f>
-        <v>.</v>
-      </c>
-      <c r="L26" s="7">
-        <f t="shared" ref="L26" si="15">IF(SUM(L24:L25) + IF(OR(SUM(M24:M25)=2,AND(SUM(M24:M25)=1,M26=0)), 1, 0) &lt; 2, SUM(L24:L25) + IF(OR(SUM(M24:M25)=2,AND(SUM(M24:M25)=1,M26=0)), 1, 0), SUM(L24:L25) + IF(OR(SUM(M24:M25)=2,AND(SUM(M24:M25)=1,M26=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="M26" s="7">
-        <f t="shared" ref="M26" si="16">IF(SUM(M24:M25) + IF(OR(SUM(N24:N25)=2,AND(SUM(N24:N25)=1,N26=0)), 1, 0) &lt; 2, SUM(M24:M25) + IF(OR(SUM(N24:N25)=2,AND(SUM(N24:N25)=1,N26=0)), 1, 0), SUM(M24:M25) + IF(OR(SUM(N24:N25)=2,AND(SUM(N24:N25)=1,N26=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="N26" s="7">
+      <c r="K26" s="3" t="str">
+        <f t="shared" ref="K26:U26" si="16">K12</f>
+        <v>.</v>
+      </c>
+      <c r="L26" s="3">
+        <f t="shared" ref="L26" si="17">IF(SUM(L24:L25) + IF(OR(SUM(M24:M25)=2,AND(SUM(M24:M25)=1,M26=0)), 1, 0) &lt; 2, SUM(L24:L25) + IF(OR(SUM(M24:M25)=2,AND(SUM(M24:M25)=1,M26=0)), 1, 0), SUM(L24:L25) + IF(OR(SUM(M24:M25)=2,AND(SUM(M24:M25)=1,M26=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="3">
+        <f t="shared" ref="M26" si="18">IF(SUM(M24:M25) + IF(OR(SUM(N24:N25)=2,AND(SUM(N24:N25)=1,N26=0)), 1, 0) &lt; 2, SUM(M24:M25) + IF(OR(SUM(N24:N25)=2,AND(SUM(N24:N25)=1,N26=0)), 1, 0), SUM(M24:M25) + IF(OR(SUM(N24:N25)=2,AND(SUM(N24:N25)=1,N26=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="3">
         <f>IF(SUM(N24:N25) + IF(OR(SUM(O24:O25)=2,AND(SUM(O24:O25)=1,O26=0)), 1, 0) &lt; 2, SUM(N24:N25) + IF(OR(SUM(O24:O25)=2,AND(SUM(O24:O25)=1,O26=0)), 1, 0), SUM(N24:N25) + IF(OR(SUM(O24:O25)=2,AND(SUM(O24:O25)=1,O26=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="O26" s="7">
+      <c r="O26" s="3">
         <f>IF(SUM(O24:O25) + IF(OR(SUM(Q24:Q25)=2,AND(SUM(Q24:Q25)=1,Q26=0)), 1, 0) &lt; 2, SUM(O24:O25) + IF(OR(SUM(Q24:Q25)=2,AND(SUM(Q24:Q25)=1,Q26=0)), 1, 0), SUM(O24:O25) + IF(OR(SUM(Q24:Q25)=2,AND(SUM(Q24:Q25)=1,Q26=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="P26" s="7" t="str">
-        <f t="shared" si="14"/>
-        <v>.</v>
-      </c>
-      <c r="Q26" s="7">
-        <f t="shared" ref="Q26" si="17">IF(SUM(Q24:Q25) + IF(OR(SUM(R24:R25)=2,AND(SUM(R24:R25)=1,R26=0)), 1, 0) &lt; 2, SUM(Q24:Q25) + IF(OR(SUM(R24:R25)=2,AND(SUM(R24:R25)=1,R26=0)), 1, 0), SUM(Q24:Q25) + IF(OR(SUM(R24:R25)=2,AND(SUM(R24:R25)=1,R26=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="R26" s="7">
-        <f t="shared" ref="R26" si="18">IF(SUM(R24:R25) + IF(OR(SUM(S24:S25)=2,AND(SUM(S24:S25)=1,S26=0)), 1, 0) &lt; 2, SUM(R24:R25) + IF(OR(SUM(S24:S25)=2,AND(SUM(S24:S25)=1,S26=0)), 1, 0), SUM(R24:R25) + IF(OR(SUM(S24:S25)=2,AND(SUM(S24:S25)=1,S26=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="S26" s="7">
+      <c r="P26" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>.</v>
+      </c>
+      <c r="Q26" s="3">
+        <f t="shared" ref="Q26" si="19">IF(SUM(Q24:Q25) + IF(OR(SUM(R24:R25)=2,AND(SUM(R24:R25)=1,R26=0)), 1, 0) &lt; 2, SUM(Q24:Q25) + IF(OR(SUM(R24:R25)=2,AND(SUM(R24:R25)=1,R26=0)), 1, 0), SUM(Q24:Q25) + IF(OR(SUM(R24:R25)=2,AND(SUM(R24:R25)=1,R26=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="3">
+        <f t="shared" ref="R26" si="20">IF(SUM(R24:R25) + IF(OR(SUM(S24:S25)=2,AND(SUM(S24:S25)=1,S26=0)), 1, 0) &lt; 2, SUM(R24:R25) + IF(OR(SUM(S24:S25)=2,AND(SUM(S24:S25)=1,S26=0)), 1, 0), SUM(R24:R25) + IF(OR(SUM(S24:S25)=2,AND(SUM(S24:S25)=1,S26=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="S26" s="3">
         <f>IF(SUM(S24:S25) + IF(OR(SUM(T24:T25)=2,AND(SUM(T24:T25)=1,T26=0)), 1, 0) &lt; 2, SUM(S24:S25) + IF(OR(SUM(T24:T25)=2,AND(SUM(T24:T25)=1,T26=0)), 1, 0), SUM(S24:S25) + IF(OR(SUM(T24:T25)=2,AND(SUM(T24:T25)=1,T26=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="T26" s="7">
+      <c r="T26" s="3">
         <f>IF(SUM(T24:T25) + IF(OR(SUM(V24:V25)=2,AND(SUM(V24:V25)=1,V26=0)), 1, 0) &lt; 2, SUM(T24:T25) + IF(OR(SUM(V24:V25)=2,AND(SUM(V24:V25)=1,V26=0)), 1, 0), SUM(T24:T25) + IF(OR(SUM(V24:V25)=2,AND(SUM(V24:V25)=1,V26=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="U26" s="7" t="str">
-        <f t="shared" si="14"/>
-        <v>.</v>
-      </c>
-      <c r="V26" s="7">
-        <f t="shared" ref="V26" si="19">IF(SUM(V24:V25) + IF(OR(SUM(W24:W25)=2,AND(SUM(W24:W25)=1,W26=0)), 1, 0) &lt; 2, SUM(V24:V25) + IF(OR(SUM(W24:W25)=2,AND(SUM(W24:W25)=1,W26=0)), 1, 0), SUM(V24:V25) + IF(OR(SUM(W24:W25)=2,AND(SUM(W24:W25)=1,W26=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="W26" s="7">
-        <f t="shared" ref="W26" si="20">IF(SUM(W24:W25) + IF(OR(SUM(X24:X25)=2,AND(SUM(X24:X25)=1,X26=0)), 1, 0) &lt; 2, SUM(W24:W25) + IF(OR(SUM(X24:X25)=2,AND(SUM(X24:X25)=1,X26=0)), 1, 0), SUM(W24:W25) + IF(OR(SUM(X24:X25)=2,AND(SUM(X24:X25)=1,X26=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="X26" s="7">
+      <c r="U26" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>.</v>
+      </c>
+      <c r="V26" s="3">
+        <f t="shared" ref="V26" si="21">IF(SUM(V24:V25) + IF(OR(SUM(W24:W25)=2,AND(SUM(W24:W25)=1,W26=0)), 1, 0) &lt; 2, SUM(V24:V25) + IF(OR(SUM(W24:W25)=2,AND(SUM(W24:W25)=1,W26=0)), 1, 0), SUM(V24:V25) + IF(OR(SUM(W24:W25)=2,AND(SUM(W24:W25)=1,W26=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="W26" s="3">
+        <f t="shared" ref="W26" si="22">IF(SUM(W24:W25) + IF(OR(SUM(X24:X25)=2,AND(SUM(X24:X25)=1,X26=0)), 1, 0) &lt; 2, SUM(W24:W25) + IF(OR(SUM(X24:X25)=2,AND(SUM(X24:X25)=1,X26=0)), 1, 0), SUM(W24:W25) + IF(OR(SUM(X24:X25)=2,AND(SUM(X24:X25)=1,X26=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="X26" s="3">
         <f>IF(SUM(X24:X25) + IF(OR(SUM(Y24:Y25)=2,AND(SUM(Y24:Y25)=1,Y26=0)), 1, 0) &lt; 2, SUM(X24:X25) + IF(OR(SUM(Y24:Y25)=2,AND(SUM(Y24:Y25)=1,Y26=0)), 1, 0), SUM(X24:X25) + IF(OR(SUM(Y24:Y25)=2,AND(SUM(Y24:Y25)=1,Y26=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="Y26" s="7">
+      <c r="Y26" s="3">
         <f>2 - (Y24 + Y25)</f>
         <v>0</v>
       </c>
@@ -3312,22 +3366,22 @@
         <f>AE24 + AE25</f>
         <v>53302</v>
       </c>
-      <c r="AG26" s="6"/>
-      <c r="AH26" s="6"/>
-      <c r="AI26" s="6"/>
-      <c r="AJ26" s="6"/>
-      <c r="AK26" s="6"/>
+      <c r="AG26" s="7"/>
+      <c r="AH26" s="7"/>
+      <c r="AI26" s="7"/>
+      <c r="AJ26" s="7"/>
+      <c r="AK26" s="7"/>
     </row>
     <row r="27" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C27" s="9"/>
-      <c r="AG27" s="6"/>
-      <c r="AH27" s="6"/>
-      <c r="AI27" s="6"/>
-      <c r="AJ27" s="6"/>
-      <c r="AK27" s="6"/>
+      <c r="C27" s="5"/>
+      <c r="AG27" s="7"/>
+      <c r="AH27" s="7"/>
+      <c r="AI27" s="7"/>
+      <c r="AJ27" s="7"/>
+      <c r="AK27" s="7"/>
     </row>
     <row r="28" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C28" s="9"/>
+      <c r="C28" s="5"/>
       <c r="F28" t="s">
         <v>59</v>
       </c>
@@ -3335,38 +3389,38 @@
         <f>IF(OR(SUM(G24:G25)=2,AND(SUM(G24:G25)=1,G26=0)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
       <c r="L28">
         <f>IF(ISEVEN(SUM(Q26:Y26)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="N28" s="5" t="s">
+      <c r="N28" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
       <c r="Q28">
         <f>IF(OR(SUM(V24:V25)=2,AND(SUM(V24:V25)=1,V26=0)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="S28" s="5" t="s">
+      <c r="S28" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="T28" s="5"/>
-      <c r="U28" s="5"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
       <c r="V28">
         <f>IF(SUM(G26:Y26)=0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="X28" s="5" t="s">
+      <c r="X28" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="Y28" s="5"/>
-      <c r="Z28" s="5"/>
+      <c r="Y28" s="8"/>
+      <c r="Z28" s="8"/>
       <c r="AA28">
         <f>G26</f>
         <v>1</v>
@@ -3378,99 +3432,99 @@
         <f>IF(OR(SUM(G24:G25)=2,AND(SUM(G24:G25)=1,G26=0)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="AG28" s="6"/>
-      <c r="AH28" s="6"/>
-      <c r="AI28" s="6"/>
-      <c r="AJ28" s="6"/>
-      <c r="AK28" s="6"/>
+      <c r="AG28" s="7"/>
+      <c r="AH28" s="7"/>
+      <c r="AI28" s="7"/>
+      <c r="AJ28" s="7"/>
+      <c r="AK28" s="7"/>
     </row>
     <row r="30" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C30" s="9">
+      <c r="C30" s="5">
         <v>3</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F30" t="s">
         <v>32</v>
       </c>
       <c r="G30">
-        <f t="shared" ref="G30:X30" si="21">G5</f>
+        <f t="shared" ref="G30:X30" si="23">G5</f>
         <v>0</v>
       </c>
       <c r="H30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="I30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="J30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>.</v>
       </c>
       <c r="L30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="M30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="N30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="O30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="P30" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>.</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="R30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="S30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="T30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U30" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>.</v>
       </c>
       <c r="V30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="W30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="X30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="Y30">
         <f>Y5</f>
         <v>1</v>
       </c>
-      <c r="AC30" s="4" t="s">
+      <c r="AC30" s="6" t="s">
         <v>57</v>
       </c>
       <c r="AD30" t="s">
@@ -3480,97 +3534,97 @@
         <f>C5</f>
         <v>25449</v>
       </c>
-      <c r="AG30" s="6" t="s">
+      <c r="AG30" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="AH30" s="6"/>
-      <c r="AI30" s="6"/>
-      <c r="AJ30" s="6"/>
-      <c r="AK30" s="6"/>
+      <c r="AH30" s="7"/>
+      <c r="AI30" s="7"/>
+      <c r="AJ30" s="7"/>
+      <c r="AK30" s="7"/>
     </row>
     <row r="31" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C31" s="9"/>
-      <c r="E31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="E31" s="6"/>
       <c r="F31" t="s">
         <v>34</v>
       </c>
       <c r="G31">
-        <f t="shared" ref="G31:X31" si="22">G10</f>
+        <f t="shared" ref="G31:X31" si="24">G10</f>
         <v>1</v>
       </c>
       <c r="H31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="I31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="J31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>.</v>
       </c>
       <c r="L31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="N31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="O31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="P31" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>.</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="R31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="S31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="T31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="U31" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>.</v>
       </c>
       <c r="V31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="W31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="X31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Y31">
         <f>Y10</f>
         <v>0</v>
       </c>
-      <c r="AC31" s="4"/>
+      <c r="AC31" s="6"/>
       <c r="AD31" t="s">
         <v>6</v>
       </c>
@@ -3578,87 +3632,87 @@
         <f>C10</f>
         <v>-2404</v>
       </c>
-      <c r="AG31" s="6"/>
-      <c r="AH31" s="6"/>
-      <c r="AI31" s="6"/>
-      <c r="AJ31" s="6"/>
-      <c r="AK31" s="6"/>
+      <c r="AG31" s="7"/>
+      <c r="AH31" s="7"/>
+      <c r="AI31" s="7"/>
+      <c r="AJ31" s="7"/>
+      <c r="AK31" s="7"/>
     </row>
     <row r="32" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C32" s="9"/>
-      <c r="G32" s="7">
-        <f t="shared" ref="G32" si="23">IF(SUM(G30:G31) + IF(OR(SUM(H30:H31)=2,AND(SUM(H30:H31)=1,H32=0)), 1, 0) &lt; 2, SUM(G30:G31) + IF(OR(SUM(H30:H31)=2,AND(SUM(H30:H31)=1,H32=0)), 1, 0), SUM(G30:G31) + IF(OR(SUM(H30:H31)=2,AND(SUM(H30:H31)=1,H32=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="7">
+      <c r="C32" s="5"/>
+      <c r="G32" s="3">
+        <f t="shared" ref="G32" si="25">IF(SUM(G30:G31) + IF(OR(SUM(H30:H31)=2,AND(SUM(H30:H31)=1,H32=0)), 1, 0) &lt; 2, SUM(G30:G31) + IF(OR(SUM(H30:H31)=2,AND(SUM(H30:H31)=1,H32=0)), 1, 0), SUM(G30:G31) + IF(OR(SUM(H30:H31)=2,AND(SUM(H30:H31)=1,H32=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="3">
         <f>IF(SUM(H30:H31) + IF(OR(SUM(I30:I31)=2,AND(SUM(I30:I31)=1,I32=0)), 1, 0) &lt; 2, SUM(H30:H31) + IF(OR(SUM(I30:I31)=2,AND(SUM(I30:I31)=1,I32=0)), 1, 0), SUM(H30:H31) + IF(OR(SUM(I30:I31)=2,AND(SUM(I30:I31)=1,I32=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="3">
         <f>IF(SUM(I30:I31) + IF(OR(SUM(J30:J31)=2,AND(SUM(J30:J31)=1,J32=0)), 1, 0) &lt; 2, SUM(I30:I31) + IF(OR(SUM(J30:J31)=2,AND(SUM(J30:J31)=1,J32=0)), 1, 0), SUM(I30:I31) + IF(OR(SUM(J30:J31)=2,AND(SUM(J30:J31)=1,J32=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="J32" s="7">
+      <c r="J32" s="3">
         <f>IF(SUM(J30:J31) + IF(OR(SUM(L30:L31)=2,AND(SUM(L30:L31)=1,L32=0)), 1, 0) &lt; 2, SUM(J30:J31) + IF(OR(SUM(L30:L31)=2,AND(SUM(L30:L31)=1,L32=0)), 1, 0), SUM(J30:J31) + IF(OR(SUM(L30:L31)=2,AND(SUM(L30:L31)=1,L32=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="K32" s="7" t="str">
-        <f t="shared" ref="K32:Y32" si="24">K18</f>
-        <v>.</v>
-      </c>
-      <c r="L32" s="7">
-        <f t="shared" ref="L32" si="25">IF(SUM(L30:L31) + IF(OR(SUM(M30:M31)=2,AND(SUM(M30:M31)=1,M32=0)), 1, 0) &lt; 2, SUM(L30:L31) + IF(OR(SUM(M30:M31)=2,AND(SUM(M30:M31)=1,M32=0)), 1, 0), SUM(L30:L31) + IF(OR(SUM(M30:M31)=2,AND(SUM(M30:M31)=1,M32=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="M32" s="7">
-        <f t="shared" ref="M32" si="26">IF(SUM(M30:M31) + IF(OR(SUM(N30:N31)=2,AND(SUM(N30:N31)=1,N32=0)), 1, 0) &lt; 2, SUM(M30:M31) + IF(OR(SUM(N30:N31)=2,AND(SUM(N30:N31)=1,N32=0)), 1, 0), SUM(M30:M31) + IF(OR(SUM(N30:N31)=2,AND(SUM(N30:N31)=1,N32=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="N32" s="7">
+      <c r="K32" s="3" t="str">
+        <f t="shared" ref="K32" si="26">K18</f>
+        <v>.</v>
+      </c>
+      <c r="L32" s="3">
+        <f t="shared" ref="L32" si="27">IF(SUM(L30:L31) + IF(OR(SUM(M30:M31)=2,AND(SUM(M30:M31)=1,M32=0)), 1, 0) &lt; 2, SUM(L30:L31) + IF(OR(SUM(M30:M31)=2,AND(SUM(M30:M31)=1,M32=0)), 1, 0), SUM(L30:L31) + IF(OR(SUM(M30:M31)=2,AND(SUM(M30:M31)=1,M32=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="M32" s="3">
+        <f t="shared" ref="M32" si="28">IF(SUM(M30:M31) + IF(OR(SUM(N30:N31)=2,AND(SUM(N30:N31)=1,N32=0)), 1, 0) &lt; 2, SUM(M30:M31) + IF(OR(SUM(N30:N31)=2,AND(SUM(N30:N31)=1,N32=0)), 1, 0), SUM(M30:M31) + IF(OR(SUM(N30:N31)=2,AND(SUM(N30:N31)=1,N32=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="3">
         <f>IF(SUM(N30:N31) + IF(OR(SUM(O30:O31)=2,AND(SUM(O30:O31)=1,O32=0)), 1, 0) &lt; 2, SUM(N30:N31) + IF(OR(SUM(O30:O31)=2,AND(SUM(O30:O31)=1,O32=0)), 1, 0), SUM(N30:N31) + IF(OR(SUM(O30:O31)=2,AND(SUM(O30:O31)=1,O32=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="O32" s="7">
+      <c r="O32" s="3">
         <f>IF(SUM(O30:O31) + IF(OR(SUM(Q30:Q31)=2,AND(SUM(Q30:Q31)=1,Q32=0)), 1, 0) &lt; 2, SUM(O30:O31) + IF(OR(SUM(Q30:Q31)=2,AND(SUM(Q30:Q31)=1,Q32=0)), 1, 0), SUM(O30:O31) + IF(OR(SUM(Q30:Q31)=2,AND(SUM(Q30:Q31)=1,Q32=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="P32" s="7" t="str">
-        <f t="shared" ref="P32:AD32" si="27">P18</f>
-        <v>.</v>
-      </c>
-      <c r="Q32" s="7">
-        <f t="shared" ref="Q32" si="28">IF(SUM(Q30:Q31) + IF(OR(SUM(R30:R31)=2,AND(SUM(R30:R31)=1,R32=0)), 1, 0) &lt; 2, SUM(Q30:Q31) + IF(OR(SUM(R30:R31)=2,AND(SUM(R30:R31)=1,R32=0)), 1, 0), SUM(Q30:Q31) + IF(OR(SUM(R30:R31)=2,AND(SUM(R30:R31)=1,R32=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="R32" s="7">
-        <f t="shared" ref="R32" si="29">IF(SUM(R30:R31) + IF(OR(SUM(S30:S31)=2,AND(SUM(S30:S31)=1,S32=0)), 1, 0) &lt; 2, SUM(R30:R31) + IF(OR(SUM(S30:S31)=2,AND(SUM(S30:S31)=1,S32=0)), 1, 0), SUM(R30:R31) + IF(OR(SUM(S30:S31)=2,AND(SUM(S30:S31)=1,S32=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="S32" s="7">
+      <c r="P32" s="3" t="str">
+        <f t="shared" ref="P32" si="29">P18</f>
+        <v>.</v>
+      </c>
+      <c r="Q32" s="3">
+        <f t="shared" ref="Q32" si="30">IF(SUM(Q30:Q31) + IF(OR(SUM(R30:R31)=2,AND(SUM(R30:R31)=1,R32=0)), 1, 0) &lt; 2, SUM(Q30:Q31) + IF(OR(SUM(R30:R31)=2,AND(SUM(R30:R31)=1,R32=0)), 1, 0), SUM(Q30:Q31) + IF(OR(SUM(R30:R31)=2,AND(SUM(R30:R31)=1,R32=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="R32" s="3">
+        <f t="shared" ref="R32" si="31">IF(SUM(R30:R31) + IF(OR(SUM(S30:S31)=2,AND(SUM(S30:S31)=1,S32=0)), 1, 0) &lt; 2, SUM(R30:R31) + IF(OR(SUM(S30:S31)=2,AND(SUM(S30:S31)=1,S32=0)), 1, 0), SUM(R30:R31) + IF(OR(SUM(S30:S31)=2,AND(SUM(S30:S31)=1,S32=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="S32" s="3">
         <f>IF(SUM(S30:S31) + IF(OR(SUM(T30:T31)=2,AND(SUM(T30:T31)=1,T32=0)), 1, 0) &lt; 2, SUM(S30:S31) + IF(OR(SUM(T30:T31)=2,AND(SUM(T30:T31)=1,T32=0)), 1, 0), SUM(S30:S31) + IF(OR(SUM(T30:T31)=2,AND(SUM(T30:T31)=1,T32=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="T32" s="7">
+      <c r="T32" s="3">
         <f>IF(SUM(T30:T31) + IF(OR(SUM(V30:V31)=2,AND(SUM(V30:V31)=1,V32=0)), 1, 0) &lt; 2, SUM(T30:T31) + IF(OR(SUM(V30:V31)=2,AND(SUM(V30:V31)=1,V32=0)), 1, 0), SUM(T30:T31) + IF(OR(SUM(V30:V31)=2,AND(SUM(V30:V31)=1,V32=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="U32" s="7" t="str">
-        <f t="shared" ref="U32:AI32" si="30">U18</f>
-        <v>.</v>
-      </c>
-      <c r="V32" s="7">
-        <f t="shared" ref="V32" si="31">IF(SUM(V30:V31) + IF(OR(SUM(W30:W31)=2,AND(SUM(W30:W31)=1,W32=0)), 1, 0) &lt; 2, SUM(V30:V31) + IF(OR(SUM(W30:W31)=2,AND(SUM(W30:W31)=1,W32=0)), 1, 0), SUM(V30:V31) + IF(OR(SUM(W30:W31)=2,AND(SUM(W30:W31)=1,W32=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="W32" s="7">
-        <f t="shared" ref="W32" si="32">IF(SUM(W30:W31) + IF(OR(SUM(X30:X31)=2,AND(SUM(X30:X31)=1,X32=0)), 1, 0) &lt; 2, SUM(W30:W31) + IF(OR(SUM(X30:X31)=2,AND(SUM(X30:X31)=1,X32=0)), 1, 0), SUM(W30:W31) + IF(OR(SUM(X30:X31)=2,AND(SUM(X30:X31)=1,X32=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="X32" s="7">
+      <c r="U32" s="3" t="str">
+        <f t="shared" ref="U32" si="32">U18</f>
+        <v>.</v>
+      </c>
+      <c r="V32" s="3">
+        <f t="shared" ref="V32" si="33">IF(SUM(V30:V31) + IF(OR(SUM(W30:W31)=2,AND(SUM(W30:W31)=1,W32=0)), 1, 0) &lt; 2, SUM(V30:V31) + IF(OR(SUM(W30:W31)=2,AND(SUM(W30:W31)=1,W32=0)), 1, 0), SUM(V30:V31) + IF(OR(SUM(W30:W31)=2,AND(SUM(W30:W31)=1,W32=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="W32" s="3">
+        <f t="shared" ref="W32" si="34">IF(SUM(W30:W31) + IF(OR(SUM(X30:X31)=2,AND(SUM(X30:X31)=1,X32=0)), 1, 0) &lt; 2, SUM(W30:W31) + IF(OR(SUM(X30:X31)=2,AND(SUM(X30:X31)=1,X32=0)), 1, 0), SUM(W30:W31) + IF(OR(SUM(X30:X31)=2,AND(SUM(X30:X31)=1,X32=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="X32" s="3">
         <f>IF(SUM(X30:X31) + IF(OR(SUM(Y30:Y31)=2,AND(SUM(Y30:Y31)=1,Y32=0)), 1, 0) &lt; 2, SUM(X30:X31) + IF(OR(SUM(Y30:Y31)=2,AND(SUM(Y30:Y31)=1,Y32=0)), 1, 0), SUM(X30:X31) + IF(OR(SUM(Y30:Y31)=2,AND(SUM(Y30:Y31)=1,Y32=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="Y32" s="7">
+      <c r="Y32" s="3">
         <f>2 - (Y30 + Y31)</f>
         <v>1</v>
       </c>
@@ -3672,22 +3726,22 @@
         <f>AE30 + AE31</f>
         <v>23045</v>
       </c>
-      <c r="AG32" s="6"/>
-      <c r="AH32" s="6"/>
-      <c r="AI32" s="6"/>
-      <c r="AJ32" s="6"/>
-      <c r="AK32" s="6"/>
+      <c r="AG32" s="7"/>
+      <c r="AH32" s="7"/>
+      <c r="AI32" s="7"/>
+      <c r="AJ32" s="7"/>
+      <c r="AK32" s="7"/>
     </row>
     <row r="33" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C33" s="9"/>
-      <c r="AG33" s="6"/>
-      <c r="AH33" s="6"/>
-      <c r="AI33" s="6"/>
-      <c r="AJ33" s="6"/>
-      <c r="AK33" s="6"/>
+      <c r="C33" s="5"/>
+      <c r="AG33" s="7"/>
+      <c r="AH33" s="7"/>
+      <c r="AI33" s="7"/>
+      <c r="AJ33" s="7"/>
+      <c r="AK33" s="7"/>
     </row>
     <row r="34" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C34" s="9"/>
+      <c r="C34" s="5"/>
       <c r="F34" t="s">
         <v>59</v>
       </c>
@@ -3695,38 +3749,38 @@
         <f>IF(OR(SUM(G30:G31)=2,AND(SUM(G30:G31)=1,G32=0)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="I34" s="5" t="s">
+      <c r="I34" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
       <c r="L34">
         <f>IF(ISEVEN(SUM(Q32:Y32)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="N34" s="5" t="s">
+      <c r="N34" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
       <c r="Q34">
         <f>IF(OR(SUM(V30:V31)=2,AND(SUM(V30:V31)=1,V32=0)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="S34" s="5" t="s">
+      <c r="S34" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="T34" s="5"/>
-      <c r="U34" s="5"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
       <c r="V34">
         <f>IF(SUM(G32:Y32)=0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="X34" s="5" t="s">
+      <c r="X34" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="Y34" s="5"/>
-      <c r="Z34" s="5"/>
+      <c r="Y34" s="8"/>
+      <c r="Z34" s="8"/>
       <c r="AA34">
         <f>G32</f>
         <v>0</v>
@@ -3738,17 +3792,17 @@
         <f>IF(OR(SUM(G30:G31)=2,AND(SUM(G30:G31)=1,G32=0)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="AG34" s="6"/>
-      <c r="AH34" s="6"/>
-      <c r="AI34" s="6"/>
-      <c r="AJ34" s="6"/>
-      <c r="AK34" s="6"/>
+      <c r="AG34" s="7"/>
+      <c r="AH34" s="7"/>
+      <c r="AI34" s="7"/>
+      <c r="AJ34" s="7"/>
+      <c r="AK34" s="7"/>
     </row>
     <row r="36" spans="3:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="9">
+      <c r="C36" s="5">
         <v>4</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F36" t="s">
@@ -3759,78 +3813,78 @@
         <v>1</v>
       </c>
       <c r="H36">
-        <f t="shared" ref="H36:Y36" si="33">H10</f>
+        <f t="shared" ref="H36:Y36" si="35">H10</f>
         <v>1</v>
       </c>
       <c r="I36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="J36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="K36" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>.</v>
       </c>
       <c r="L36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="M36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="N36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="O36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="P36" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>.</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="R36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="S36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="T36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="U36" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>.</v>
       </c>
       <c r="V36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="W36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="X36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="Y36">
-        <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="AC36" s="4" t="s">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="AC36" s="6" t="s">
         <v>57</v>
       </c>
       <c r="AD36" t="s">
@@ -3840,17 +3894,17 @@
         <f>C10</f>
         <v>-2404</v>
       </c>
-      <c r="AG36" s="6" t="s">
+      <c r="AG36" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AH36" s="6"/>
-      <c r="AI36" s="6"/>
-      <c r="AJ36" s="6"/>
-      <c r="AK36" s="6"/>
+      <c r="AH36" s="7"/>
+      <c r="AI36" s="7"/>
+      <c r="AJ36" s="7"/>
+      <c r="AK36" s="7"/>
     </row>
     <row r="37" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C37" s="9"/>
-      <c r="E37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="E37" s="6"/>
       <c r="F37" t="s">
         <v>35</v>
       </c>
@@ -3859,166 +3913,166 @@
         <v>1</v>
       </c>
       <c r="H37">
-        <f t="shared" ref="H37:Y37" si="34">H11</f>
+        <f t="shared" ref="H37:Y37" si="36">H11</f>
         <v>0</v>
       </c>
       <c r="I37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="J37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1</v>
       </c>
       <c r="K37" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>.</v>
       </c>
       <c r="L37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1</v>
       </c>
       <c r="M37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1</v>
       </c>
       <c r="N37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="P37" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>.</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1</v>
       </c>
       <c r="R37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="S37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="T37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1</v>
       </c>
       <c r="U37" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>.</v>
       </c>
       <c r="V37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="W37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1</v>
       </c>
       <c r="X37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1</v>
       </c>
       <c r="Y37">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="AC37" s="4"/>
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="AC37" s="6"/>
       <c r="AD37" t="s">
         <v>7</v>
       </c>
-      <c r="AE37" s="8">
+      <c r="AE37" s="4">
         <f>C11</f>
         <v>-25449</v>
       </c>
-      <c r="AG37" s="6"/>
-      <c r="AH37" s="6"/>
-      <c r="AI37" s="6"/>
-      <c r="AJ37" s="6"/>
-      <c r="AK37" s="6"/>
+      <c r="AG37" s="7"/>
+      <c r="AH37" s="7"/>
+      <c r="AI37" s="7"/>
+      <c r="AJ37" s="7"/>
+      <c r="AK37" s="7"/>
     </row>
     <row r="38" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C38" s="9"/>
-      <c r="G38" s="7">
-        <f t="shared" ref="G38" si="35">IF(SUM(G36:G37) + IF(OR(SUM(H36:H37)=2,AND(SUM(H36:H37)=1,H38=0)), 1, 0) &lt; 2, SUM(G36:G37) + IF(OR(SUM(H36:H37)=2,AND(SUM(H36:H37)=1,H38=0)), 1, 0), SUM(G36:G37) + IF(OR(SUM(H36:H37)=2,AND(SUM(H36:H37)=1,H38=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="H38" s="7">
+      <c r="C38" s="5"/>
+      <c r="G38" s="3">
+        <f t="shared" ref="G38" si="37">IF(SUM(G36:G37) + IF(OR(SUM(H36:H37)=2,AND(SUM(H36:H37)=1,H38=0)), 1, 0) &lt; 2, SUM(G36:G37) + IF(OR(SUM(H36:H37)=2,AND(SUM(H36:H37)=1,H38=0)), 1, 0), SUM(G36:G37) + IF(OR(SUM(H36:H37)=2,AND(SUM(H36:H37)=1,H38=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="H38" s="3">
         <f>IF(SUM(H36:H37) + IF(OR(SUM(I36:I37)=2,AND(SUM(I36:I37)=1,I38=0)), 1, 0) &lt; 2, SUM(H36:H37) + IF(OR(SUM(I36:I37)=2,AND(SUM(I36:I37)=1,I38=0)), 1, 0), SUM(H36:H37) + IF(OR(SUM(I36:I37)=2,AND(SUM(I36:I37)=1,I38=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="I38" s="7">
+      <c r="I38" s="3">
         <f>IF(SUM(I36:I37) + IF(OR(SUM(J36:J37)=2,AND(SUM(J36:J37)=1,J38=0)), 1, 0) &lt; 2, SUM(I36:I37) + IF(OR(SUM(J36:J37)=2,AND(SUM(J36:J37)=1,J38=0)), 1, 0), SUM(I36:I37) + IF(OR(SUM(J36:J37)=2,AND(SUM(J36:J37)=1,J38=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="J38" s="7">
+      <c r="J38" s="3">
         <f>IF(SUM(J36:J37) + IF(OR(SUM(L36:L37)=2,AND(SUM(L36:L37)=1,L38=0)), 1, 0) &lt; 2, SUM(J36:J37) + IF(OR(SUM(L36:L37)=2,AND(SUM(L36:L37)=1,L38=0)), 1, 0), SUM(J36:J37) + IF(OR(SUM(L36:L37)=2,AND(SUM(L36:L37)=1,L38=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="K38" s="7" t="str">
-        <f t="shared" ref="K38:Y38" si="36">K24</f>
-        <v>.</v>
-      </c>
-      <c r="L38" s="7">
-        <f t="shared" ref="L38" si="37">IF(SUM(L36:L37) + IF(OR(SUM(M36:M37)=2,AND(SUM(M36:M37)=1,M38=0)), 1, 0) &lt; 2, SUM(L36:L37) + IF(OR(SUM(M36:M37)=2,AND(SUM(M36:M37)=1,M38=0)), 1, 0), SUM(L36:L37) + IF(OR(SUM(M36:M37)=2,AND(SUM(M36:M37)=1,M38=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="M38" s="7">
-        <f t="shared" ref="M38" si="38">IF(SUM(M36:M37) + IF(OR(SUM(N36:N37)=2,AND(SUM(N36:N37)=1,N38=0)), 1, 0) &lt; 2, SUM(M36:M37) + IF(OR(SUM(N36:N37)=2,AND(SUM(N36:N37)=1,N38=0)), 1, 0), SUM(M36:M37) + IF(OR(SUM(N36:N37)=2,AND(SUM(N36:N37)=1,N38=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="N38" s="7">
+      <c r="K38" s="3" t="str">
+        <f t="shared" ref="K38" si="38">K24</f>
+        <v>.</v>
+      </c>
+      <c r="L38" s="3">
+        <f t="shared" ref="L38" si="39">IF(SUM(L36:L37) + IF(OR(SUM(M36:M37)=2,AND(SUM(M36:M37)=1,M38=0)), 1, 0) &lt; 2, SUM(L36:L37) + IF(OR(SUM(M36:M37)=2,AND(SUM(M36:M37)=1,M38=0)), 1, 0), SUM(L36:L37) + IF(OR(SUM(M36:M37)=2,AND(SUM(M36:M37)=1,M38=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="M38" s="3">
+        <f t="shared" ref="M38" si="40">IF(SUM(M36:M37) + IF(OR(SUM(N36:N37)=2,AND(SUM(N36:N37)=1,N38=0)), 1, 0) &lt; 2, SUM(M36:M37) + IF(OR(SUM(N36:N37)=2,AND(SUM(N36:N37)=1,N38=0)), 1, 0), SUM(M36:M37) + IF(OR(SUM(N36:N37)=2,AND(SUM(N36:N37)=1,N38=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="3">
         <f>IF(SUM(N36:N37) + IF(OR(SUM(O36:O37)=2,AND(SUM(O36:O37)=1,O38=0)), 1, 0) &lt; 2, SUM(N36:N37) + IF(OR(SUM(O36:O37)=2,AND(SUM(O36:O37)=1,O38=0)), 1, 0), SUM(N36:N37) + IF(OR(SUM(O36:O37)=2,AND(SUM(O36:O37)=1,O38=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="O38" s="7">
+      <c r="O38" s="3">
         <f>IF(SUM(O36:O37) + IF(OR(SUM(Q36:Q37)=2,AND(SUM(Q36:Q37)=1,Q38=0)), 1, 0) &lt; 2, SUM(O36:O37) + IF(OR(SUM(Q36:Q37)=2,AND(SUM(Q36:Q37)=1,Q38=0)), 1, 0), SUM(O36:O37) + IF(OR(SUM(Q36:Q37)=2,AND(SUM(Q36:Q37)=1,Q38=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="P38" s="7" t="str">
-        <f t="shared" ref="P38:AD38" si="39">P24</f>
-        <v>.</v>
-      </c>
-      <c r="Q38" s="7">
-        <f t="shared" ref="Q38" si="40">IF(SUM(Q36:Q37) + IF(OR(SUM(R36:R37)=2,AND(SUM(R36:R37)=1,R38=0)), 1, 0) &lt; 2, SUM(Q36:Q37) + IF(OR(SUM(R36:R37)=2,AND(SUM(R36:R37)=1,R38=0)), 1, 0), SUM(Q36:Q37) + IF(OR(SUM(R36:R37)=2,AND(SUM(R36:R37)=1,R38=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="R38" s="7">
-        <f t="shared" ref="R38" si="41">IF(SUM(R36:R37) + IF(OR(SUM(S36:S37)=2,AND(SUM(S36:S37)=1,S38=0)), 1, 0) &lt; 2, SUM(R36:R37) + IF(OR(SUM(S36:S37)=2,AND(SUM(S36:S37)=1,S38=0)), 1, 0), SUM(R36:R37) + IF(OR(SUM(S36:S37)=2,AND(SUM(S36:S37)=1,S38=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="S38" s="7">
+      <c r="P38" s="3" t="str">
+        <f t="shared" ref="P38" si="41">P24</f>
+        <v>.</v>
+      </c>
+      <c r="Q38" s="3">
+        <f t="shared" ref="Q38" si="42">IF(SUM(Q36:Q37) + IF(OR(SUM(R36:R37)=2,AND(SUM(R36:R37)=1,R38=0)), 1, 0) &lt; 2, SUM(Q36:Q37) + IF(OR(SUM(R36:R37)=2,AND(SUM(R36:R37)=1,R38=0)), 1, 0), SUM(Q36:Q37) + IF(OR(SUM(R36:R37)=2,AND(SUM(R36:R37)=1,R38=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="R38" s="3">
+        <f t="shared" ref="R38" si="43">IF(SUM(R36:R37) + IF(OR(SUM(S36:S37)=2,AND(SUM(S36:S37)=1,S38=0)), 1, 0) &lt; 2, SUM(R36:R37) + IF(OR(SUM(S36:S37)=2,AND(SUM(S36:S37)=1,S38=0)), 1, 0), SUM(R36:R37) + IF(OR(SUM(S36:S37)=2,AND(SUM(S36:S37)=1,S38=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="S38" s="3">
         <f>IF(SUM(S36:S37) + IF(OR(SUM(T36:T37)=2,AND(SUM(T36:T37)=1,T38=0)), 1, 0) &lt; 2, SUM(S36:S37) + IF(OR(SUM(T36:T37)=2,AND(SUM(T36:T37)=1,T38=0)), 1, 0), SUM(S36:S37) + IF(OR(SUM(T36:T37)=2,AND(SUM(T36:T37)=1,T38=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="T38" s="7">
+      <c r="T38" s="3">
         <f>IF(SUM(T36:T37) + IF(OR(SUM(V36:V37)=2,AND(SUM(V36:V37)=1,V38=0)), 1, 0) &lt; 2, SUM(T36:T37) + IF(OR(SUM(V36:V37)=2,AND(SUM(V36:V37)=1,V38=0)), 1, 0), SUM(T36:T37) + IF(OR(SUM(V36:V37)=2,AND(SUM(V36:V37)=1,V38=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="U38" s="7" t="str">
-        <f t="shared" ref="U38:AI38" si="42">U24</f>
-        <v>.</v>
-      </c>
-      <c r="V38" s="7">
-        <f t="shared" ref="V38" si="43">IF(SUM(V36:V37) + IF(OR(SUM(W36:W37)=2,AND(SUM(W36:W37)=1,W38=0)), 1, 0) &lt; 2, SUM(V36:V37) + IF(OR(SUM(W36:W37)=2,AND(SUM(W36:W37)=1,W38=0)), 1, 0), SUM(V36:V37) + IF(OR(SUM(W36:W37)=2,AND(SUM(W36:W37)=1,W38=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="W38" s="7">
-        <f t="shared" ref="W38" si="44">IF(SUM(W36:W37) + IF(OR(SUM(X36:X37)=2,AND(SUM(X36:X37)=1,X38=0)), 1, 0) &lt; 2, SUM(W36:W37) + IF(OR(SUM(X36:X37)=2,AND(SUM(X36:X37)=1,X38=0)), 1, 0), SUM(W36:W37) + IF(OR(SUM(X36:X37)=2,AND(SUM(X36:X37)=1,X38=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="X38" s="7">
+      <c r="U38" s="3" t="str">
+        <f t="shared" ref="U38" si="44">U24</f>
+        <v>.</v>
+      </c>
+      <c r="V38" s="3">
+        <f t="shared" ref="V38" si="45">IF(SUM(V36:V37) + IF(OR(SUM(W36:W37)=2,AND(SUM(W36:W37)=1,W38=0)), 1, 0) &lt; 2, SUM(V36:V37) + IF(OR(SUM(W36:W37)=2,AND(SUM(W36:W37)=1,W38=0)), 1, 0), SUM(V36:V37) + IF(OR(SUM(W36:W37)=2,AND(SUM(W36:W37)=1,W38=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="W38" s="3">
+        <f t="shared" ref="W38" si="46">IF(SUM(W36:W37) + IF(OR(SUM(X36:X37)=2,AND(SUM(X36:X37)=1,X38=0)), 1, 0) &lt; 2, SUM(W36:W37) + IF(OR(SUM(X36:X37)=2,AND(SUM(X36:X37)=1,X38=0)), 1, 0), SUM(W36:W37) + IF(OR(SUM(X36:X37)=2,AND(SUM(X36:X37)=1,X38=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="X38" s="3">
         <f>IF(SUM(X36:X37) + IF(OR(SUM(Y36:Y37)=2,AND(SUM(Y36:Y37)=1,Y38=0)), 1, 0) &lt; 2, SUM(X36:X37) + IF(OR(SUM(Y36:Y37)=2,AND(SUM(Y36:Y37)=1,Y38=0)), 1, 0), SUM(X36:X37) + IF(OR(SUM(Y36:Y37)=2,AND(SUM(Y36:Y37)=1,Y38=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="Y38" s="7">
+      <c r="Y38" s="3">
         <f>2 - (Y36 + Y37)</f>
         <v>1</v>
       </c>
@@ -4032,22 +4086,22 @@
         <f>AE36 + AE37</f>
         <v>-27853</v>
       </c>
-      <c r="AG38" s="6"/>
-      <c r="AH38" s="6"/>
-      <c r="AI38" s="6"/>
-      <c r="AJ38" s="6"/>
-      <c r="AK38" s="6"/>
+      <c r="AG38" s="7"/>
+      <c r="AH38" s="7"/>
+      <c r="AI38" s="7"/>
+      <c r="AJ38" s="7"/>
+      <c r="AK38" s="7"/>
     </row>
     <row r="39" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C39" s="9"/>
-      <c r="AG39" s="6"/>
-      <c r="AH39" s="6"/>
-      <c r="AI39" s="6"/>
-      <c r="AJ39" s="6"/>
-      <c r="AK39" s="6"/>
+      <c r="C39" s="5"/>
+      <c r="AG39" s="7"/>
+      <c r="AH39" s="7"/>
+      <c r="AI39" s="7"/>
+      <c r="AJ39" s="7"/>
+      <c r="AK39" s="7"/>
     </row>
     <row r="40" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C40" s="9"/>
+      <c r="C40" s="5"/>
       <c r="F40" t="s">
         <v>59</v>
       </c>
@@ -4055,38 +4109,38 @@
         <f>IF(OR(SUM(G36:G37)=2,AND(SUM(G36:G37)=1,G38=0)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="I40" s="5" t="s">
+      <c r="I40" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
       <c r="L40">
         <f>IF(ISEVEN(SUM(Q38:Y38)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="N40" s="5" t="s">
+      <c r="N40" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
       <c r="Q40">
         <f>IF(OR(SUM(V36:V37)=2,AND(SUM(V36:V37)=1,V38=0)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="S40" s="5" t="s">
+      <c r="S40" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="T40" s="5"/>
-      <c r="U40" s="5"/>
+      <c r="T40" s="8"/>
+      <c r="U40" s="8"/>
       <c r="V40">
         <f>IF(SUM(G38:Y38)=0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="X40" s="5" t="s">
+      <c r="X40" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="Y40" s="5"/>
-      <c r="Z40" s="5"/>
+      <c r="Y40" s="8"/>
+      <c r="Z40" s="8"/>
       <c r="AA40">
         <f>G38</f>
         <v>1</v>
@@ -4098,17 +4152,17 @@
         <f>IF(OR(SUM(G36:G37)=2,AND(SUM(G36:G37)=1,G38=0)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="AG40" s="6"/>
-      <c r="AH40" s="6"/>
-      <c r="AI40" s="6"/>
-      <c r="AJ40" s="6"/>
-      <c r="AK40" s="6"/>
+      <c r="AG40" s="7"/>
+      <c r="AH40" s="7"/>
+      <c r="AI40" s="7"/>
+      <c r="AJ40" s="7"/>
+      <c r="AK40" s="7"/>
     </row>
     <row r="42" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C42" s="9">
+      <c r="C42" s="5">
         <v>5</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F42" t="s">
@@ -4119,78 +4173,78 @@
         <v>1</v>
       </c>
       <c r="H42">
-        <f t="shared" ref="H42:Y42" si="45">H11</f>
+        <f t="shared" ref="H42:Y42" si="47">H11</f>
         <v>0</v>
       </c>
       <c r="I42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="J42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>1</v>
       </c>
       <c r="K42" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>.</v>
       </c>
       <c r="L42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>1</v>
       </c>
       <c r="M42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>1</v>
       </c>
       <c r="N42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="O42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="P42" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>.</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>1</v>
       </c>
       <c r="R42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="S42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="T42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>1</v>
       </c>
       <c r="U42" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>.</v>
       </c>
       <c r="V42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="W42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>1</v>
       </c>
       <c r="X42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>1</v>
       </c>
       <c r="Y42">
-        <f t="shared" si="45"/>
-        <v>1</v>
-      </c>
-      <c r="AC42" s="4" t="s">
+        <f t="shared" si="47"/>
+        <v>1</v>
+      </c>
+      <c r="AC42" s="6" t="s">
         <v>57</v>
       </c>
       <c r="AD42" t="s">
@@ -4200,17 +4254,17 @@
         <f>C11</f>
         <v>-25449</v>
       </c>
-      <c r="AG42" s="6" t="s">
+      <c r="AG42" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AH42" s="6"/>
-      <c r="AI42" s="6"/>
-      <c r="AJ42" s="6"/>
-      <c r="AK42" s="6"/>
+      <c r="AH42" s="7"/>
+      <c r="AI42" s="7"/>
+      <c r="AJ42" s="7"/>
+      <c r="AK42" s="7"/>
     </row>
     <row r="43" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C43" s="9"/>
-      <c r="E43" s="4"/>
+      <c r="C43" s="5"/>
+      <c r="E43" s="6"/>
       <c r="F43" t="s">
         <v>36</v>
       </c>
@@ -4219,166 +4273,166 @@
         <v>1</v>
       </c>
       <c r="H43">
-        <f t="shared" ref="H43:Y43" si="46">H12</f>
+        <f t="shared" ref="H43:Y43" si="48">H12</f>
         <v>0</v>
       </c>
       <c r="I43">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="J43">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1</v>
       </c>
       <c r="K43" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>.</v>
       </c>
       <c r="L43">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="M43">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="N43">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1</v>
       </c>
       <c r="O43">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1</v>
       </c>
       <c r="P43" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>.</v>
       </c>
       <c r="Q43">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="R43">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="S43">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1</v>
       </c>
       <c r="T43">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1</v>
       </c>
       <c r="U43" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>.</v>
       </c>
       <c r="V43">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W43">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="X43">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>1</v>
       </c>
       <c r="Y43">
-        <f t="shared" si="46"/>
-        <v>1</v>
-      </c>
-      <c r="AC43" s="4"/>
+        <f t="shared" si="48"/>
+        <v>1</v>
+      </c>
+      <c r="AC43" s="6"/>
       <c r="AD43" t="s">
         <v>8</v>
       </c>
-      <c r="AE43" s="8">
+      <c r="AE43" s="4">
         <f>C12</f>
         <v>-27853</v>
       </c>
-      <c r="AG43" s="6"/>
-      <c r="AH43" s="6"/>
-      <c r="AI43" s="6"/>
-      <c r="AJ43" s="6"/>
-      <c r="AK43" s="6"/>
+      <c r="AG43" s="7"/>
+      <c r="AH43" s="7"/>
+      <c r="AI43" s="7"/>
+      <c r="AJ43" s="7"/>
+      <c r="AK43" s="7"/>
     </row>
     <row r="44" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C44" s="9"/>
-      <c r="G44" s="7">
-        <f t="shared" ref="G44" si="47">IF(SUM(G42:G43) + IF(OR(SUM(H42:H43)=2,AND(SUM(H42:H43)=1,H44=0)), 1, 0) &lt; 2, SUM(G42:G43) + IF(OR(SUM(H42:H43)=2,AND(SUM(H42:H43)=1,H44=0)), 1, 0), SUM(G42:G43) + IF(OR(SUM(H42:H43)=2,AND(SUM(H42:H43)=1,H44=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="H44" s="7">
+      <c r="C44" s="5"/>
+      <c r="G44" s="3">
+        <f t="shared" ref="G44" si="49">IF(SUM(G42:G43) + IF(OR(SUM(H42:H43)=2,AND(SUM(H42:H43)=1,H44=0)), 1, 0) &lt; 2, SUM(G42:G43) + IF(OR(SUM(H42:H43)=2,AND(SUM(H42:H43)=1,H44=0)), 1, 0), SUM(G42:G43) + IF(OR(SUM(H42:H43)=2,AND(SUM(H42:H43)=1,H44=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="H44" s="3">
         <f>IF(SUM(H42:H43) + IF(OR(SUM(I42:I43)=2,AND(SUM(I42:I43)=1,I44=0)), 1, 0) &lt; 2, SUM(H42:H43) + IF(OR(SUM(I42:I43)=2,AND(SUM(I42:I43)=1,I44=0)), 1, 0), SUM(H42:H43) + IF(OR(SUM(I42:I43)=2,AND(SUM(I42:I43)=1,I44=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="I44" s="7">
+      <c r="I44" s="3">
         <f>IF(SUM(I42:I43) + IF(OR(SUM(J42:J43)=2,AND(SUM(J42:J43)=1,J44=0)), 1, 0) &lt; 2, SUM(I42:I43) + IF(OR(SUM(J42:J43)=2,AND(SUM(J42:J43)=1,J44=0)), 1, 0), SUM(I42:I43) + IF(OR(SUM(J42:J43)=2,AND(SUM(J42:J43)=1,J44=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="J44" s="7">
+      <c r="J44" s="3">
         <f>IF(SUM(J42:J43) + IF(OR(SUM(L42:L43)=2,AND(SUM(L42:L43)=1,L44=0)), 1, 0) &lt; 2, SUM(J42:J43) + IF(OR(SUM(L42:L43)=2,AND(SUM(L42:L43)=1,L44=0)), 1, 0), SUM(J42:J43) + IF(OR(SUM(L42:L43)=2,AND(SUM(L42:L43)=1,L44=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="K44" s="7" t="str">
-        <f t="shared" ref="K44:Y44" si="48">K30</f>
-        <v>.</v>
-      </c>
-      <c r="L44" s="7">
-        <f t="shared" ref="L44" si="49">IF(SUM(L42:L43) + IF(OR(SUM(M42:M43)=2,AND(SUM(M42:M43)=1,M44=0)), 1, 0) &lt; 2, SUM(L42:L43) + IF(OR(SUM(M42:M43)=2,AND(SUM(M42:M43)=1,M44=0)), 1, 0), SUM(L42:L43) + IF(OR(SUM(M42:M43)=2,AND(SUM(M42:M43)=1,M44=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="M44" s="7">
-        <f t="shared" ref="M44" si="50">IF(SUM(M42:M43) + IF(OR(SUM(N42:N43)=2,AND(SUM(N42:N43)=1,N44=0)), 1, 0) &lt; 2, SUM(M42:M43) + IF(OR(SUM(N42:N43)=2,AND(SUM(N42:N43)=1,N44=0)), 1, 0), SUM(M42:M43) + IF(OR(SUM(N42:N43)=2,AND(SUM(N42:N43)=1,N44=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="N44" s="7">
+      <c r="K44" s="3" t="str">
+        <f t="shared" ref="K44" si="50">K30</f>
+        <v>.</v>
+      </c>
+      <c r="L44" s="3">
+        <f t="shared" ref="L44" si="51">IF(SUM(L42:L43) + IF(OR(SUM(M42:M43)=2,AND(SUM(M42:M43)=1,M44=0)), 1, 0) &lt; 2, SUM(L42:L43) + IF(OR(SUM(M42:M43)=2,AND(SUM(M42:M43)=1,M44=0)), 1, 0), SUM(L42:L43) + IF(OR(SUM(M42:M43)=2,AND(SUM(M42:M43)=1,M44=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="M44" s="3">
+        <f t="shared" ref="M44" si="52">IF(SUM(M42:M43) + IF(OR(SUM(N42:N43)=2,AND(SUM(N42:N43)=1,N44=0)), 1, 0) &lt; 2, SUM(M42:M43) + IF(OR(SUM(N42:N43)=2,AND(SUM(N42:N43)=1,N44=0)), 1, 0), SUM(M42:M43) + IF(OR(SUM(N42:N43)=2,AND(SUM(N42:N43)=1,N44=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="N44" s="3">
         <f>IF(SUM(N42:N43) + IF(OR(SUM(O42:O43)=2,AND(SUM(O42:O43)=1,O44=0)), 1, 0) &lt; 2, SUM(N42:N43) + IF(OR(SUM(O42:O43)=2,AND(SUM(O42:O43)=1,O44=0)), 1, 0), SUM(N42:N43) + IF(OR(SUM(O42:O43)=2,AND(SUM(O42:O43)=1,O44=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="O44" s="7">
+      <c r="O44" s="3">
         <f>IF(SUM(O42:O43) + IF(OR(SUM(Q42:Q43)=2,AND(SUM(Q42:Q43)=1,Q44=0)), 1, 0) &lt; 2, SUM(O42:O43) + IF(OR(SUM(Q42:Q43)=2,AND(SUM(Q42:Q43)=1,Q44=0)), 1, 0), SUM(O42:O43) + IF(OR(SUM(Q42:Q43)=2,AND(SUM(Q42:Q43)=1,Q44=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="P44" s="7" t="str">
-        <f t="shared" ref="P44:AD44" si="51">P30</f>
-        <v>.</v>
-      </c>
-      <c r="Q44" s="7">
-        <f t="shared" ref="Q44" si="52">IF(SUM(Q42:Q43) + IF(OR(SUM(R42:R43)=2,AND(SUM(R42:R43)=1,R44=0)), 1, 0) &lt; 2, SUM(Q42:Q43) + IF(OR(SUM(R42:R43)=2,AND(SUM(R42:R43)=1,R44=0)), 1, 0), SUM(Q42:Q43) + IF(OR(SUM(R42:R43)=2,AND(SUM(R42:R43)=1,R44=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="R44" s="7">
-        <f t="shared" ref="R44" si="53">IF(SUM(R42:R43) + IF(OR(SUM(S42:S43)=2,AND(SUM(S42:S43)=1,S44=0)), 1, 0) &lt; 2, SUM(R42:R43) + IF(OR(SUM(S42:S43)=2,AND(SUM(S42:S43)=1,S44=0)), 1, 0), SUM(R42:R43) + IF(OR(SUM(S42:S43)=2,AND(SUM(S42:S43)=1,S44=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="S44" s="7">
+      <c r="P44" s="3" t="str">
+        <f t="shared" ref="P44" si="53">P30</f>
+        <v>.</v>
+      </c>
+      <c r="Q44" s="3">
+        <f t="shared" ref="Q44" si="54">IF(SUM(Q42:Q43) + IF(OR(SUM(R42:R43)=2,AND(SUM(R42:R43)=1,R44=0)), 1, 0) &lt; 2, SUM(Q42:Q43) + IF(OR(SUM(R42:R43)=2,AND(SUM(R42:R43)=1,R44=0)), 1, 0), SUM(Q42:Q43) + IF(OR(SUM(R42:R43)=2,AND(SUM(R42:R43)=1,R44=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="R44" s="3">
+        <f t="shared" ref="R44" si="55">IF(SUM(R42:R43) + IF(OR(SUM(S42:S43)=2,AND(SUM(S42:S43)=1,S44=0)), 1, 0) &lt; 2, SUM(R42:R43) + IF(OR(SUM(S42:S43)=2,AND(SUM(S42:S43)=1,S44=0)), 1, 0), SUM(R42:R43) + IF(OR(SUM(S42:S43)=2,AND(SUM(S42:S43)=1,S44=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="S44" s="3">
         <f>IF(SUM(S42:S43) + IF(OR(SUM(T42:T43)=2,AND(SUM(T42:T43)=1,T44=0)), 1, 0) &lt; 2, SUM(S42:S43) + IF(OR(SUM(T42:T43)=2,AND(SUM(T42:T43)=1,T44=0)), 1, 0), SUM(S42:S43) + IF(OR(SUM(T42:T43)=2,AND(SUM(T42:T43)=1,T44=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="T44" s="7">
+      <c r="T44" s="3">
         <f>IF(SUM(T42:T43) + IF(OR(SUM(V42:V43)=2,AND(SUM(V42:V43)=1,V44=0)), 1, 0) &lt; 2, SUM(T42:T43) + IF(OR(SUM(V42:V43)=2,AND(SUM(V42:V43)=1,V44=0)), 1, 0), SUM(T42:T43) + IF(OR(SUM(V42:V43)=2,AND(SUM(V42:V43)=1,V44=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="U44" s="7" t="str">
-        <f t="shared" ref="U44:AI44" si="54">U30</f>
-        <v>.</v>
-      </c>
-      <c r="V44" s="7">
-        <f t="shared" ref="V44" si="55">IF(SUM(V42:V43) + IF(OR(SUM(W42:W43)=2,AND(SUM(W42:W43)=1,W44=0)), 1, 0) &lt; 2, SUM(V42:V43) + IF(OR(SUM(W42:W43)=2,AND(SUM(W42:W43)=1,W44=0)), 1, 0), SUM(V42:V43) + IF(OR(SUM(W42:W43)=2,AND(SUM(W42:W43)=1,W44=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="W44" s="7">
-        <f t="shared" ref="W44" si="56">IF(SUM(W42:W43) + IF(OR(SUM(X42:X43)=2,AND(SUM(X42:X43)=1,X44=0)), 1, 0) &lt; 2, SUM(W42:W43) + IF(OR(SUM(X42:X43)=2,AND(SUM(X42:X43)=1,X44=0)), 1, 0), SUM(W42:W43) + IF(OR(SUM(X42:X43)=2,AND(SUM(X42:X43)=1,X44=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="X44" s="7">
+      <c r="U44" s="3" t="str">
+        <f t="shared" ref="U44" si="56">U30</f>
+        <v>.</v>
+      </c>
+      <c r="V44" s="3">
+        <f t="shared" ref="V44" si="57">IF(SUM(V42:V43) + IF(OR(SUM(W42:W43)=2,AND(SUM(W42:W43)=1,W44=0)), 1, 0) &lt; 2, SUM(V42:V43) + IF(OR(SUM(W42:W43)=2,AND(SUM(W42:W43)=1,W44=0)), 1, 0), SUM(V42:V43) + IF(OR(SUM(W42:W43)=2,AND(SUM(W42:W43)=1,W44=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="W44" s="3">
+        <f t="shared" ref="W44" si="58">IF(SUM(W42:W43) + IF(OR(SUM(X42:X43)=2,AND(SUM(X42:X43)=1,X44=0)), 1, 0) &lt; 2, SUM(W42:W43) + IF(OR(SUM(X42:X43)=2,AND(SUM(X42:X43)=1,X44=0)), 1, 0), SUM(W42:W43) + IF(OR(SUM(X42:X43)=2,AND(SUM(X42:X43)=1,X44=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="X44" s="3">
         <f>IF(SUM(X42:X43) + IF(OR(SUM(Y42:Y43)=2,AND(SUM(Y42:Y43)=1,Y44=0)), 1, 0) &lt; 2, SUM(X42:X43) + IF(OR(SUM(Y42:Y43)=2,AND(SUM(Y42:Y43)=1,Y44=0)), 1, 0), SUM(X42:X43) + IF(OR(SUM(Y42:Y43)=2,AND(SUM(Y42:Y43)=1,Y44=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="Y44" s="7">
+      <c r="Y44" s="3">
         <f>2 - (Y42 + Y43)</f>
         <v>0</v>
       </c>
@@ -4392,22 +4446,22 @@
         <f>AE42 + AE43</f>
         <v>-53302</v>
       </c>
-      <c r="AG44" s="6"/>
-      <c r="AH44" s="6"/>
-      <c r="AI44" s="6"/>
-      <c r="AJ44" s="6"/>
-      <c r="AK44" s="6"/>
+      <c r="AG44" s="7"/>
+      <c r="AH44" s="7"/>
+      <c r="AI44" s="7"/>
+      <c r="AJ44" s="7"/>
+      <c r="AK44" s="7"/>
     </row>
     <row r="45" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C45" s="9"/>
-      <c r="AG45" s="6"/>
-      <c r="AH45" s="6"/>
-      <c r="AI45" s="6"/>
-      <c r="AJ45" s="6"/>
-      <c r="AK45" s="6"/>
+      <c r="C45" s="5"/>
+      <c r="AG45" s="7"/>
+      <c r="AH45" s="7"/>
+      <c r="AI45" s="7"/>
+      <c r="AJ45" s="7"/>
+      <c r="AK45" s="7"/>
     </row>
     <row r="46" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C46" s="9"/>
+      <c r="C46" s="5"/>
       <c r="F46" t="s">
         <v>59</v>
       </c>
@@ -4415,38 +4469,38 @@
         <f>IF(OR(SUM(G42:G43)=2,AND(SUM(G42:G43)=1,G44=0)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="I46" s="5" t="s">
+      <c r="I46" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
       <c r="L46">
         <f>IF(ISEVEN(SUM(Q44:Y44)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="N46" s="5" t="s">
+      <c r="N46" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="O46" s="5"/>
-      <c r="P46" s="5"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
       <c r="Q46">
         <f>IF(OR(SUM(V42:V43)=2,AND(SUM(V42:V43)=1,V44=0)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="S46" s="5" t="s">
+      <c r="S46" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="T46" s="5"/>
-      <c r="U46" s="5"/>
+      <c r="T46" s="8"/>
+      <c r="U46" s="8"/>
       <c r="V46">
         <f>IF(SUM(G44:Y44)=0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="X46" s="5" t="s">
+      <c r="X46" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="Y46" s="5"/>
-      <c r="Z46" s="5"/>
+      <c r="Y46" s="8"/>
+      <c r="Z46" s="8"/>
       <c r="AA46">
         <f>G44</f>
         <v>0</v>
@@ -4458,17 +4512,17 @@
         <f>IF(OR(SUM(G42:G43)=2,AND(SUM(G42:G43)=1,G44=0)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="AG46" s="6"/>
-      <c r="AH46" s="6"/>
-      <c r="AI46" s="6"/>
-      <c r="AJ46" s="6"/>
-      <c r="AK46" s="6"/>
+      <c r="AG46" s="7"/>
+      <c r="AH46" s="7"/>
+      <c r="AI46" s="7"/>
+      <c r="AJ46" s="7"/>
+      <c r="AK46" s="7"/>
     </row>
     <row r="48" spans="3:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="9">
+      <c r="C48" s="5">
         <v>6</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F48" t="s">
@@ -4479,78 +4533,78 @@
         <v>0</v>
       </c>
       <c r="H48">
-        <f t="shared" ref="H48:Y48" si="57">H4</f>
+        <f t="shared" ref="H48:Y48" si="59">H4</f>
         <v>0</v>
       </c>
       <c r="I48">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="J48">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="K48" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>.</v>
       </c>
       <c r="L48">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>1</v>
       </c>
       <c r="M48">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="N48">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="O48">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>1</v>
       </c>
       <c r="P48" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>.</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="R48">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>1</v>
       </c>
       <c r="S48">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>1</v>
       </c>
       <c r="T48">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="U48" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>.</v>
       </c>
       <c r="V48">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="W48">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>1</v>
       </c>
       <c r="X48">
-        <f t="shared" si="57"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="Y48">
-        <f t="shared" si="57"/>
-        <v>0</v>
-      </c>
-      <c r="AC48" s="4" t="s">
+        <f t="shared" si="59"/>
+        <v>0</v>
+      </c>
+      <c r="AC48" s="6" t="s">
         <v>57</v>
       </c>
       <c r="AD48" t="s">
@@ -4560,17 +4614,17 @@
         <f>C4</f>
         <v>2404</v>
       </c>
-      <c r="AG48" s="6" t="s">
+      <c r="AG48" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AH48" s="6"/>
-      <c r="AI48" s="6"/>
-      <c r="AJ48" s="6"/>
-      <c r="AK48" s="6"/>
+      <c r="AH48" s="7"/>
+      <c r="AI48" s="7"/>
+      <c r="AJ48" s="7"/>
+      <c r="AK48" s="7"/>
     </row>
     <row r="49" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C49" s="9"/>
-      <c r="E49" s="4"/>
+      <c r="C49" s="5"/>
+      <c r="E49" s="6"/>
       <c r="F49" t="s">
         <v>35</v>
       </c>
@@ -4579,166 +4633,166 @@
         <v>1</v>
       </c>
       <c r="H49">
-        <f t="shared" ref="H49:Y49" si="58">H11</f>
+        <f t="shared" ref="H49:Y49" si="60">H11</f>
         <v>0</v>
       </c>
       <c r="I49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="J49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>1</v>
       </c>
       <c r="K49" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>.</v>
       </c>
       <c r="L49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>1</v>
       </c>
       <c r="M49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>1</v>
       </c>
       <c r="N49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="O49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="P49" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>.</v>
       </c>
       <c r="Q49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>1</v>
       </c>
       <c r="R49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="S49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="T49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>1</v>
       </c>
       <c r="U49" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>.</v>
       </c>
       <c r="V49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="W49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>1</v>
       </c>
       <c r="X49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>1</v>
       </c>
       <c r="Y49">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="AC49" s="4"/>
+        <f t="shared" si="60"/>
+        <v>1</v>
+      </c>
+      <c r="AC49" s="6"/>
       <c r="AD49" t="s">
         <v>7</v>
       </c>
-      <c r="AE49" s="8">
+      <c r="AE49" s="4">
         <f>C11</f>
         <v>-25449</v>
       </c>
-      <c r="AG49" s="6"/>
-      <c r="AH49" s="6"/>
-      <c r="AI49" s="6"/>
-      <c r="AJ49" s="6"/>
-      <c r="AK49" s="6"/>
+      <c r="AG49" s="7"/>
+      <c r="AH49" s="7"/>
+      <c r="AI49" s="7"/>
+      <c r="AJ49" s="7"/>
+      <c r="AK49" s="7"/>
     </row>
     <row r="50" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C50" s="9"/>
-      <c r="G50" s="7">
-        <f t="shared" ref="G50" si="59">IF(SUM(G48:G49) + IF(OR(SUM(H48:H49)=2,AND(SUM(H48:H49)=1,H50=0)), 1, 0) &lt; 2, SUM(G48:G49) + IF(OR(SUM(H48:H49)=2,AND(SUM(H48:H49)=1,H50=0)), 1, 0), SUM(G48:G49) + IF(OR(SUM(H48:H49)=2,AND(SUM(H48:H49)=1,H50=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="H50" s="7">
+      <c r="C50" s="5"/>
+      <c r="G50" s="3">
+        <f t="shared" ref="G50" si="61">IF(SUM(G48:G49) + IF(OR(SUM(H48:H49)=2,AND(SUM(H48:H49)=1,H50=0)), 1, 0) &lt; 2, SUM(G48:G49) + IF(OR(SUM(H48:H49)=2,AND(SUM(H48:H49)=1,H50=0)), 1, 0), SUM(G48:G49) + IF(OR(SUM(H48:H49)=2,AND(SUM(H48:H49)=1,H50=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="H50" s="3">
         <f>IF(SUM(H48:H49) + IF(OR(SUM(I48:I49)=2,AND(SUM(I48:I49)=1,I50=0)), 1, 0) &lt; 2, SUM(H48:H49) + IF(OR(SUM(I48:I49)=2,AND(SUM(I48:I49)=1,I50=0)), 1, 0), SUM(H48:H49) + IF(OR(SUM(I48:I49)=2,AND(SUM(I48:I49)=1,I50=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="I50" s="7">
+      <c r="I50" s="3">
         <f>IF(SUM(I48:I49) + IF(OR(SUM(J48:J49)=2,AND(SUM(J48:J49)=1,J50=0)), 1, 0) &lt; 2, SUM(I48:I49) + IF(OR(SUM(J48:J49)=2,AND(SUM(J48:J49)=1,J50=0)), 1, 0), SUM(I48:I49) + IF(OR(SUM(J48:J49)=2,AND(SUM(J48:J49)=1,J50=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="J50" s="7">
+      <c r="J50" s="3">
         <f>IF(SUM(J48:J49) + IF(OR(SUM(L48:L49)=2,AND(SUM(L48:L49)=1,L50=0)), 1, 0) &lt; 2, SUM(J48:J49) + IF(OR(SUM(L48:L49)=2,AND(SUM(L48:L49)=1,L50=0)), 1, 0), SUM(J48:J49) + IF(OR(SUM(L48:L49)=2,AND(SUM(L48:L49)=1,L50=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="K50" s="7" t="str">
-        <f t="shared" ref="K50:Y50" si="60">K36</f>
-        <v>.</v>
-      </c>
-      <c r="L50" s="7">
-        <f t="shared" ref="L50" si="61">IF(SUM(L48:L49) + IF(OR(SUM(M48:M49)=2,AND(SUM(M48:M49)=1,M50=0)), 1, 0) &lt; 2, SUM(L48:L49) + IF(OR(SUM(M48:M49)=2,AND(SUM(M48:M49)=1,M50=0)), 1, 0), SUM(L48:L49) + IF(OR(SUM(M48:M49)=2,AND(SUM(M48:M49)=1,M50=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="M50" s="7">
-        <f t="shared" ref="M50" si="62">IF(SUM(M48:M49) + IF(OR(SUM(N48:N49)=2,AND(SUM(N48:N49)=1,N50=0)), 1, 0) &lt; 2, SUM(M48:M49) + IF(OR(SUM(N48:N49)=2,AND(SUM(N48:N49)=1,N50=0)), 1, 0), SUM(M48:M49) + IF(OR(SUM(N48:N49)=2,AND(SUM(N48:N49)=1,N50=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="N50" s="7">
+      <c r="K50" s="3" t="str">
+        <f t="shared" ref="K50" si="62">K36</f>
+        <v>.</v>
+      </c>
+      <c r="L50" s="3">
+        <f t="shared" ref="L50" si="63">IF(SUM(L48:L49) + IF(OR(SUM(M48:M49)=2,AND(SUM(M48:M49)=1,M50=0)), 1, 0) &lt; 2, SUM(L48:L49) + IF(OR(SUM(M48:M49)=2,AND(SUM(M48:M49)=1,M50=0)), 1, 0), SUM(L48:L49) + IF(OR(SUM(M48:M49)=2,AND(SUM(M48:M49)=1,M50=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="M50" s="3">
+        <f t="shared" ref="M50" si="64">IF(SUM(M48:M49) + IF(OR(SUM(N48:N49)=2,AND(SUM(N48:N49)=1,N50=0)), 1, 0) &lt; 2, SUM(M48:M49) + IF(OR(SUM(N48:N49)=2,AND(SUM(N48:N49)=1,N50=0)), 1, 0), SUM(M48:M49) + IF(OR(SUM(N48:N49)=2,AND(SUM(N48:N49)=1,N50=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="N50" s="3">
         <f>IF(SUM(N48:N49) + IF(OR(SUM(O48:O49)=2,AND(SUM(O48:O49)=1,O50=0)), 1, 0) &lt; 2, SUM(N48:N49) + IF(OR(SUM(O48:O49)=2,AND(SUM(O48:O49)=1,O50=0)), 1, 0), SUM(N48:N49) + IF(OR(SUM(O48:O49)=2,AND(SUM(O48:O49)=1,O50=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="O50" s="7">
+      <c r="O50" s="3">
         <f>IF(SUM(O48:O49) + IF(OR(SUM(Q48:Q49)=2,AND(SUM(Q48:Q49)=1,Q50=0)), 1, 0) &lt; 2, SUM(O48:O49) + IF(OR(SUM(Q48:Q49)=2,AND(SUM(Q48:Q49)=1,Q50=0)), 1, 0), SUM(O48:O49) + IF(OR(SUM(Q48:Q49)=2,AND(SUM(Q48:Q49)=1,Q50=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="P50" s="7" t="str">
-        <f t="shared" ref="P50:AD50" si="63">P36</f>
-        <v>.</v>
-      </c>
-      <c r="Q50" s="7">
-        <f t="shared" ref="Q50" si="64">IF(SUM(Q48:Q49) + IF(OR(SUM(R48:R49)=2,AND(SUM(R48:R49)=1,R50=0)), 1, 0) &lt; 2, SUM(Q48:Q49) + IF(OR(SUM(R48:R49)=2,AND(SUM(R48:R49)=1,R50=0)), 1, 0), SUM(Q48:Q49) + IF(OR(SUM(R48:R49)=2,AND(SUM(R48:R49)=1,R50=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="R50" s="7">
-        <f t="shared" ref="R50" si="65">IF(SUM(R48:R49) + IF(OR(SUM(S48:S49)=2,AND(SUM(S48:S49)=1,S50=0)), 1, 0) &lt; 2, SUM(R48:R49) + IF(OR(SUM(S48:S49)=2,AND(SUM(S48:S49)=1,S50=0)), 1, 0), SUM(R48:R49) + IF(OR(SUM(S48:S49)=2,AND(SUM(S48:S49)=1,S50=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="S50" s="7">
+      <c r="P50" s="3" t="str">
+        <f t="shared" ref="P50" si="65">P36</f>
+        <v>.</v>
+      </c>
+      <c r="Q50" s="3">
+        <f t="shared" ref="Q50" si="66">IF(SUM(Q48:Q49) + IF(OR(SUM(R48:R49)=2,AND(SUM(R48:R49)=1,R50=0)), 1, 0) &lt; 2, SUM(Q48:Q49) + IF(OR(SUM(R48:R49)=2,AND(SUM(R48:R49)=1,R50=0)), 1, 0), SUM(Q48:Q49) + IF(OR(SUM(R48:R49)=2,AND(SUM(R48:R49)=1,R50=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="R50" s="3">
+        <f t="shared" ref="R50" si="67">IF(SUM(R48:R49) + IF(OR(SUM(S48:S49)=2,AND(SUM(S48:S49)=1,S50=0)), 1, 0) &lt; 2, SUM(R48:R49) + IF(OR(SUM(S48:S49)=2,AND(SUM(S48:S49)=1,S50=0)), 1, 0), SUM(R48:R49) + IF(OR(SUM(S48:S49)=2,AND(SUM(S48:S49)=1,S50=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="S50" s="3">
         <f>IF(SUM(S48:S49) + IF(OR(SUM(T48:T49)=2,AND(SUM(T48:T49)=1,T50=0)), 1, 0) &lt; 2, SUM(S48:S49) + IF(OR(SUM(T48:T49)=2,AND(SUM(T48:T49)=1,T50=0)), 1, 0), SUM(S48:S49) + IF(OR(SUM(T48:T49)=2,AND(SUM(T48:T49)=1,T50=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="T50" s="7">
+      <c r="T50" s="3">
         <f>IF(SUM(T48:T49) + IF(OR(SUM(V48:V49)=2,AND(SUM(V48:V49)=1,V50=0)), 1, 0) &lt; 2, SUM(T48:T49) + IF(OR(SUM(V48:V49)=2,AND(SUM(V48:V49)=1,V50=0)), 1, 0), SUM(T48:T49) + IF(OR(SUM(V48:V49)=2,AND(SUM(V48:V49)=1,V50=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="U50" s="7" t="str">
-        <f t="shared" ref="U50:AI50" si="66">U36</f>
-        <v>.</v>
-      </c>
-      <c r="V50" s="7">
-        <f t="shared" ref="V50" si="67">IF(SUM(V48:V49) + IF(OR(SUM(W48:W49)=2,AND(SUM(W48:W49)=1,W50=0)), 1, 0) &lt; 2, SUM(V48:V49) + IF(OR(SUM(W48:W49)=2,AND(SUM(W48:W49)=1,W50=0)), 1, 0), SUM(V48:V49) + IF(OR(SUM(W48:W49)=2,AND(SUM(W48:W49)=1,W50=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="W50" s="7">
-        <f t="shared" ref="W50" si="68">IF(SUM(W48:W49) + IF(OR(SUM(X48:X49)=2,AND(SUM(X48:X49)=1,X50=0)), 1, 0) &lt; 2, SUM(W48:W49) + IF(OR(SUM(X48:X49)=2,AND(SUM(X48:X49)=1,X50=0)), 1, 0), SUM(W48:W49) + IF(OR(SUM(X48:X49)=2,AND(SUM(X48:X49)=1,X50=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="X50" s="7">
+      <c r="U50" s="3" t="str">
+        <f t="shared" ref="U50" si="68">U36</f>
+        <v>.</v>
+      </c>
+      <c r="V50" s="3">
+        <f t="shared" ref="V50" si="69">IF(SUM(V48:V49) + IF(OR(SUM(W48:W49)=2,AND(SUM(W48:W49)=1,W50=0)), 1, 0) &lt; 2, SUM(V48:V49) + IF(OR(SUM(W48:W49)=2,AND(SUM(W48:W49)=1,W50=0)), 1, 0), SUM(V48:V49) + IF(OR(SUM(W48:W49)=2,AND(SUM(W48:W49)=1,W50=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="W50" s="3">
+        <f t="shared" ref="W50" si="70">IF(SUM(W48:W49) + IF(OR(SUM(X48:X49)=2,AND(SUM(X48:X49)=1,X50=0)), 1, 0) &lt; 2, SUM(W48:W49) + IF(OR(SUM(X48:X49)=2,AND(SUM(X48:X49)=1,X50=0)), 1, 0), SUM(W48:W49) + IF(OR(SUM(X48:X49)=2,AND(SUM(X48:X49)=1,X50=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="X50" s="3">
         <f>IF(SUM(X48:X49) + IF(OR(SUM(Y48:Y49)=2,AND(SUM(Y48:Y49)=1,Y50=0)), 1, 0) &lt; 2, SUM(X48:X49) + IF(OR(SUM(Y48:Y49)=2,AND(SUM(Y48:Y49)=1,Y50=0)), 1, 0), SUM(X48:X49) + IF(OR(SUM(Y48:Y49)=2,AND(SUM(Y48:Y49)=1,Y50=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="Y50" s="7">
+      <c r="Y50" s="3">
         <f>2 - (Y48 + Y49)</f>
         <v>1</v>
       </c>
@@ -4752,22 +4806,22 @@
         <f>AE48 + AE49</f>
         <v>-23045</v>
       </c>
-      <c r="AG50" s="6"/>
-      <c r="AH50" s="6"/>
-      <c r="AI50" s="6"/>
-      <c r="AJ50" s="6"/>
-      <c r="AK50" s="6"/>
+      <c r="AG50" s="7"/>
+      <c r="AH50" s="7"/>
+      <c r="AI50" s="7"/>
+      <c r="AJ50" s="7"/>
+      <c r="AK50" s="7"/>
     </row>
     <row r="51" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C51" s="9"/>
-      <c r="AG51" s="6"/>
-      <c r="AH51" s="6"/>
-      <c r="AI51" s="6"/>
-      <c r="AJ51" s="6"/>
-      <c r="AK51" s="6"/>
+      <c r="C51" s="5"/>
+      <c r="AG51" s="7"/>
+      <c r="AH51" s="7"/>
+      <c r="AI51" s="7"/>
+      <c r="AJ51" s="7"/>
+      <c r="AK51" s="7"/>
     </row>
     <row r="52" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C52" s="9"/>
+      <c r="C52" s="5"/>
       <c r="F52" t="s">
         <v>59</v>
       </c>
@@ -4775,38 +4829,38 @@
         <f>IF(OR(SUM(G48:G49)=2,AND(SUM(G48:G49)=1,G50=0)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="I52" s="5" t="s">
+      <c r="I52" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
       <c r="L52">
         <f>IF(ISEVEN(SUM(Q50:Y50)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="N52" s="5" t="s">
+      <c r="N52" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="O52" s="5"/>
-      <c r="P52" s="5"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
       <c r="Q52">
         <f>IF(OR(SUM(V48:V49)=2,AND(SUM(V48:V49)=1,V50=0)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="S52" s="5" t="s">
+      <c r="S52" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="T52" s="5"/>
-      <c r="U52" s="5"/>
+      <c r="T52" s="8"/>
+      <c r="U52" s="8"/>
       <c r="V52">
         <f>IF(SUM(G50:Y50)=0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="X52" s="5" t="s">
+      <c r="X52" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="Y52" s="5"/>
-      <c r="Z52" s="5"/>
+      <c r="Y52" s="8"/>
+      <c r="Z52" s="8"/>
       <c r="AA52">
         <f>G50</f>
         <v>1</v>
@@ -4818,17 +4872,17 @@
         <f>IF(OR(SUM(G48:G49)=2,AND(SUM(G48:G49)=1,G50=0)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="AG52" s="6"/>
-      <c r="AH52" s="6"/>
-      <c r="AI52" s="6"/>
-      <c r="AJ52" s="6"/>
-      <c r="AK52" s="6"/>
+      <c r="AG52" s="7"/>
+      <c r="AH52" s="7"/>
+      <c r="AI52" s="7"/>
+      <c r="AJ52" s="7"/>
+      <c r="AK52" s="7"/>
     </row>
     <row r="54" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C54" s="9">
+      <c r="C54" s="5">
         <v>7</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="6" t="s">
         <v>57</v>
       </c>
       <c r="F54" t="s">
@@ -4839,78 +4893,78 @@
         <v>1</v>
       </c>
       <c r="H54">
-        <f t="shared" ref="H54:Y54" si="69">H14</f>
+        <f t="shared" ref="H54:Y54" si="71">H14</f>
         <v>0</v>
       </c>
       <c r="I54">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
       <c r="J54">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="K54" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>.</v>
       </c>
       <c r="L54">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="M54">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
       <c r="N54">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="O54">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
       <c r="P54" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>.</v>
       </c>
       <c r="Q54">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
       <c r="R54">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
       <c r="S54">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
       <c r="T54">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
       <c r="U54" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>.</v>
       </c>
       <c r="V54">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
       <c r="W54">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="X54">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
       <c r="Y54">
-        <f t="shared" si="69"/>
-        <v>1</v>
-      </c>
-      <c r="AC54" s="4" t="s">
+        <f t="shared" si="71"/>
+        <v>1</v>
+      </c>
+      <c r="AC54" s="6" t="s">
         <v>57</v>
       </c>
       <c r="AD54" t="s">
@@ -4920,17 +4974,17 @@
         <f>C14</f>
         <v>-23045</v>
       </c>
-      <c r="AG54" s="6" t="s">
+      <c r="AG54" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="AH54" s="6"/>
-      <c r="AI54" s="6"/>
-      <c r="AJ54" s="6"/>
-      <c r="AK54" s="6"/>
+      <c r="AH54" s="7"/>
+      <c r="AI54" s="7"/>
+      <c r="AJ54" s="7"/>
+      <c r="AK54" s="7"/>
     </row>
     <row r="55" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C55" s="9"/>
-      <c r="E55" s="4"/>
+      <c r="C55" s="5"/>
+      <c r="E55" s="6"/>
       <c r="F55" t="s">
         <v>33</v>
       </c>
@@ -4939,166 +4993,166 @@
         <v>0</v>
       </c>
       <c r="H55">
-        <f t="shared" ref="H55:Y55" si="70">H6</f>
+        <f t="shared" ref="H55:Y55" si="72">H6</f>
         <v>1</v>
       </c>
       <c r="I55">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>1</v>
       </c>
       <c r="J55">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="K55" t="str">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>.</v>
       </c>
       <c r="L55">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>1</v>
       </c>
       <c r="M55">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>1</v>
       </c>
       <c r="N55">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="O55">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="P55" t="str">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>.</v>
       </c>
       <c r="Q55">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>1</v>
       </c>
       <c r="R55">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>1</v>
       </c>
       <c r="S55">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="T55">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="U55" t="str">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>.</v>
       </c>
       <c r="V55">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>1</v>
       </c>
       <c r="W55">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>1</v>
       </c>
       <c r="X55">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="Y55">
-        <f t="shared" si="70"/>
-        <v>1</v>
-      </c>
-      <c r="AC55" s="4"/>
+        <f t="shared" si="72"/>
+        <v>1</v>
+      </c>
+      <c r="AC55" s="6"/>
       <c r="AD55" t="s">
         <v>5</v>
       </c>
-      <c r="AE55" s="8">
+      <c r="AE55" s="4">
         <f>C6</f>
         <v>27853</v>
       </c>
-      <c r="AG55" s="6"/>
-      <c r="AH55" s="6"/>
-      <c r="AI55" s="6"/>
-      <c r="AJ55" s="6"/>
-      <c r="AK55" s="6"/>
+      <c r="AG55" s="7"/>
+      <c r="AH55" s="7"/>
+      <c r="AI55" s="7"/>
+      <c r="AJ55" s="7"/>
+      <c r="AK55" s="7"/>
     </row>
     <row r="56" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C56" s="9"/>
-      <c r="G56" s="7">
-        <f t="shared" ref="G56" si="71">IF(SUM(G54:G55) + IF(OR(SUM(H54:H55)=2,AND(SUM(H54:H55)=1,H56=0)), 1, 0) &lt; 2, SUM(G54:G55) + IF(OR(SUM(H54:H55)=2,AND(SUM(H54:H55)=1,H56=0)), 1, 0), SUM(G54:G55) + IF(OR(SUM(H54:H55)=2,AND(SUM(H54:H55)=1,H56=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="H56" s="7">
+      <c r="C56" s="5"/>
+      <c r="G56" s="3">
+        <f t="shared" ref="G56" si="73">IF(SUM(G54:G55) + IF(OR(SUM(H54:H55)=2,AND(SUM(H54:H55)=1,H56=0)), 1, 0) &lt; 2, SUM(G54:G55) + IF(OR(SUM(H54:H55)=2,AND(SUM(H54:H55)=1,H56=0)), 1, 0), SUM(G54:G55) + IF(OR(SUM(H54:H55)=2,AND(SUM(H54:H55)=1,H56=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="H56" s="3">
         <f>IF(SUM(H54:H55) + IF(OR(SUM(I54:I55)=2,AND(SUM(I54:I55)=1,I56=0)), 1, 0) &lt; 2, SUM(H54:H55) + IF(OR(SUM(I54:I55)=2,AND(SUM(I54:I55)=1,I56=0)), 1, 0), SUM(H54:H55) + IF(OR(SUM(I54:I55)=2,AND(SUM(I54:I55)=1,I56=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="I56" s="7">
+      <c r="I56" s="3">
         <f>IF(SUM(I54:I55) + IF(OR(SUM(J54:J55)=2,AND(SUM(J54:J55)=1,J56=0)), 1, 0) &lt; 2, SUM(I54:I55) + IF(OR(SUM(J54:J55)=2,AND(SUM(J54:J55)=1,J56=0)), 1, 0), SUM(I54:I55) + IF(OR(SUM(J54:J55)=2,AND(SUM(J54:J55)=1,J56=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="J56" s="7">
+      <c r="J56" s="3">
         <f>IF(SUM(J54:J55) + IF(OR(SUM(L54:L55)=2,AND(SUM(L54:L55)=1,L56=0)), 1, 0) &lt; 2, SUM(J54:J55) + IF(OR(SUM(L54:L55)=2,AND(SUM(L54:L55)=1,L56=0)), 1, 0), SUM(J54:J55) + IF(OR(SUM(L54:L55)=2,AND(SUM(L54:L55)=1,L56=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="K56" s="7" t="str">
-        <f t="shared" ref="K56:Y56" si="72">K42</f>
-        <v>.</v>
-      </c>
-      <c r="L56" s="7">
-        <f t="shared" ref="L56" si="73">IF(SUM(L54:L55) + IF(OR(SUM(M54:M55)=2,AND(SUM(M54:M55)=1,M56=0)), 1, 0) &lt; 2, SUM(L54:L55) + IF(OR(SUM(M54:M55)=2,AND(SUM(M54:M55)=1,M56=0)), 1, 0), SUM(L54:L55) + IF(OR(SUM(M54:M55)=2,AND(SUM(M54:M55)=1,M56=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="M56" s="7">
-        <f t="shared" ref="M56" si="74">IF(SUM(M54:M55) + IF(OR(SUM(N54:N55)=2,AND(SUM(N54:N55)=1,N56=0)), 1, 0) &lt; 2, SUM(M54:M55) + IF(OR(SUM(N54:N55)=2,AND(SUM(N54:N55)=1,N56=0)), 1, 0), SUM(M54:M55) + IF(OR(SUM(N54:N55)=2,AND(SUM(N54:N55)=1,N56=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="N56" s="7">
+      <c r="K56" s="3" t="str">
+        <f t="shared" ref="K56" si="74">K42</f>
+        <v>.</v>
+      </c>
+      <c r="L56" s="3">
+        <f t="shared" ref="L56" si="75">IF(SUM(L54:L55) + IF(OR(SUM(M54:M55)=2,AND(SUM(M54:M55)=1,M56=0)), 1, 0) &lt; 2, SUM(L54:L55) + IF(OR(SUM(M54:M55)=2,AND(SUM(M54:M55)=1,M56=0)), 1, 0), SUM(L54:L55) + IF(OR(SUM(M54:M55)=2,AND(SUM(M54:M55)=1,M56=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="M56" s="3">
+        <f t="shared" ref="M56" si="76">IF(SUM(M54:M55) + IF(OR(SUM(N54:N55)=2,AND(SUM(N54:N55)=1,N56=0)), 1, 0) &lt; 2, SUM(M54:M55) + IF(OR(SUM(N54:N55)=2,AND(SUM(N54:N55)=1,N56=0)), 1, 0), SUM(M54:M55) + IF(OR(SUM(N54:N55)=2,AND(SUM(N54:N55)=1,N56=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="N56" s="3">
         <f>IF(SUM(N54:N55) + IF(OR(SUM(O54:O55)=2,AND(SUM(O54:O55)=1,O56=0)), 1, 0) &lt; 2, SUM(N54:N55) + IF(OR(SUM(O54:O55)=2,AND(SUM(O54:O55)=1,O56=0)), 1, 0), SUM(N54:N55) + IF(OR(SUM(O54:O55)=2,AND(SUM(O54:O55)=1,O56=0)), 1, 0) - 2)</f>
         <v>1</v>
       </c>
-      <c r="O56" s="7">
+      <c r="O56" s="3">
         <f>IF(SUM(O54:O55) + IF(OR(SUM(Q54:Q55)=2,AND(SUM(Q54:Q55)=1,Q56=0)), 1, 0) &lt; 2, SUM(O54:O55) + IF(OR(SUM(Q54:Q55)=2,AND(SUM(Q54:Q55)=1,Q56=0)), 1, 0), SUM(O54:O55) + IF(OR(SUM(Q54:Q55)=2,AND(SUM(Q54:Q55)=1,Q56=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="P56" s="7" t="str">
-        <f t="shared" ref="P56:AD56" si="75">P42</f>
-        <v>.</v>
-      </c>
-      <c r="Q56" s="7">
-        <f t="shared" ref="Q56" si="76">IF(SUM(Q54:Q55) + IF(OR(SUM(R54:R55)=2,AND(SUM(R54:R55)=1,R56=0)), 1, 0) &lt; 2, SUM(Q54:Q55) + IF(OR(SUM(R54:R55)=2,AND(SUM(R54:R55)=1,R56=0)), 1, 0), SUM(Q54:Q55) + IF(OR(SUM(R54:R55)=2,AND(SUM(R54:R55)=1,R56=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="R56" s="7">
-        <f t="shared" ref="R56" si="77">IF(SUM(R54:R55) + IF(OR(SUM(S54:S55)=2,AND(SUM(S54:S55)=1,S56=0)), 1, 0) &lt; 2, SUM(R54:R55) + IF(OR(SUM(S54:S55)=2,AND(SUM(S54:S55)=1,S56=0)), 1, 0), SUM(R54:R55) + IF(OR(SUM(S54:S55)=2,AND(SUM(S54:S55)=1,S56=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="S56" s="7">
+      <c r="P56" s="3" t="str">
+        <f t="shared" ref="P56" si="77">P42</f>
+        <v>.</v>
+      </c>
+      <c r="Q56" s="3">
+        <f t="shared" ref="Q56" si="78">IF(SUM(Q54:Q55) + IF(OR(SUM(R54:R55)=2,AND(SUM(R54:R55)=1,R56=0)), 1, 0) &lt; 2, SUM(Q54:Q55) + IF(OR(SUM(R54:R55)=2,AND(SUM(R54:R55)=1,R56=0)), 1, 0), SUM(Q54:Q55) + IF(OR(SUM(R54:R55)=2,AND(SUM(R54:R55)=1,R56=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="R56" s="3">
+        <f t="shared" ref="R56" si="79">IF(SUM(R54:R55) + IF(OR(SUM(S54:S55)=2,AND(SUM(S54:S55)=1,S56=0)), 1, 0) &lt; 2, SUM(R54:R55) + IF(OR(SUM(S54:S55)=2,AND(SUM(S54:S55)=1,S56=0)), 1, 0), SUM(R54:R55) + IF(OR(SUM(S54:S55)=2,AND(SUM(S54:S55)=1,S56=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="S56" s="3">
         <f>IF(SUM(S54:S55) + IF(OR(SUM(T54:T55)=2,AND(SUM(T54:T55)=1,T56=0)), 1, 0) &lt; 2, SUM(S54:S55) + IF(OR(SUM(T54:T55)=2,AND(SUM(T54:T55)=1,T56=0)), 1, 0), SUM(S54:S55) + IF(OR(SUM(T54:T55)=2,AND(SUM(T54:T55)=1,T56=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="T56" s="7">
+      <c r="T56" s="3">
         <f>IF(SUM(T54:T55) + IF(OR(SUM(V54:V55)=2,AND(SUM(V54:V55)=1,V56=0)), 1, 0) &lt; 2, SUM(T54:T55) + IF(OR(SUM(V54:V55)=2,AND(SUM(V54:V55)=1,V56=0)), 1, 0), SUM(T54:T55) + IF(OR(SUM(V54:V55)=2,AND(SUM(V54:V55)=1,V56=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="U56" s="7" t="str">
-        <f t="shared" ref="U56:AI56" si="78">U42</f>
-        <v>.</v>
-      </c>
-      <c r="V56" s="7">
-        <f t="shared" ref="V56" si="79">IF(SUM(V54:V55) + IF(OR(SUM(W54:W55)=2,AND(SUM(W54:W55)=1,W56=0)), 1, 0) &lt; 2, SUM(V54:V55) + IF(OR(SUM(W54:W55)=2,AND(SUM(W54:W55)=1,W56=0)), 1, 0), SUM(V54:V55) + IF(OR(SUM(W54:W55)=2,AND(SUM(W54:W55)=1,W56=0)), 1, 0) - 2)</f>
-        <v>1</v>
-      </c>
-      <c r="W56" s="7">
-        <f t="shared" ref="W56" si="80">IF(SUM(W54:W55) + IF(OR(SUM(X54:X55)=2,AND(SUM(X54:X55)=1,X56=0)), 1, 0) &lt; 2, SUM(W54:W55) + IF(OR(SUM(X54:X55)=2,AND(SUM(X54:X55)=1,X56=0)), 1, 0), SUM(W54:W55) + IF(OR(SUM(X54:X55)=2,AND(SUM(X54:X55)=1,X56=0)), 1, 0) - 2)</f>
-        <v>0</v>
-      </c>
-      <c r="X56" s="7">
+      <c r="U56" s="3" t="str">
+        <f t="shared" ref="U56" si="80">U42</f>
+        <v>.</v>
+      </c>
+      <c r="V56" s="3">
+        <f t="shared" ref="V56" si="81">IF(SUM(V54:V55) + IF(OR(SUM(W54:W55)=2,AND(SUM(W54:W55)=1,W56=0)), 1, 0) &lt; 2, SUM(V54:V55) + IF(OR(SUM(W54:W55)=2,AND(SUM(W54:W55)=1,W56=0)), 1, 0), SUM(V54:V55) + IF(OR(SUM(W54:W55)=2,AND(SUM(W54:W55)=1,W56=0)), 1, 0) - 2)</f>
+        <v>1</v>
+      </c>
+      <c r="W56" s="3">
+        <f t="shared" ref="W56" si="82">IF(SUM(W54:W55) + IF(OR(SUM(X54:X55)=2,AND(SUM(X54:X55)=1,X56=0)), 1, 0) &lt; 2, SUM(W54:W55) + IF(OR(SUM(X54:X55)=2,AND(SUM(X54:X55)=1,X56=0)), 1, 0), SUM(W54:W55) + IF(OR(SUM(X54:X55)=2,AND(SUM(X54:X55)=1,X56=0)), 1, 0) - 2)</f>
+        <v>0</v>
+      </c>
+      <c r="X56" s="3">
         <f>IF(SUM(X54:X55) + IF(OR(SUM(Y54:Y55)=2,AND(SUM(Y54:Y55)=1,Y56=0)), 1, 0) &lt; 2, SUM(X54:X55) + IF(OR(SUM(Y54:Y55)=2,AND(SUM(Y54:Y55)=1,Y56=0)), 1, 0), SUM(X54:X55) + IF(OR(SUM(Y54:Y55)=2,AND(SUM(Y54:Y55)=1,Y56=0)), 1, 0) - 2)</f>
         <v>0</v>
       </c>
-      <c r="Y56" s="7">
+      <c r="Y56" s="3">
         <f>2 - (Y54 + Y55)</f>
         <v>0</v>
       </c>
@@ -5112,22 +5166,22 @@
         <f>AE54 + AE55</f>
         <v>4808</v>
       </c>
-      <c r="AG56" s="6"/>
-      <c r="AH56" s="6"/>
-      <c r="AI56" s="6"/>
-      <c r="AJ56" s="6"/>
-      <c r="AK56" s="6"/>
+      <c r="AG56" s="7"/>
+      <c r="AH56" s="7"/>
+      <c r="AI56" s="7"/>
+      <c r="AJ56" s="7"/>
+      <c r="AK56" s="7"/>
     </row>
     <row r="57" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C57" s="9"/>
-      <c r="AG57" s="6"/>
-      <c r="AH57" s="6"/>
-      <c r="AI57" s="6"/>
-      <c r="AJ57" s="6"/>
-      <c r="AK57" s="6"/>
+      <c r="C57" s="5"/>
+      <c r="AG57" s="7"/>
+      <c r="AH57" s="7"/>
+      <c r="AI57" s="7"/>
+      <c r="AJ57" s="7"/>
+      <c r="AK57" s="7"/>
     </row>
     <row r="58" spans="3:37" x14ac:dyDescent="0.3">
-      <c r="C58" s="9"/>
+      <c r="C58" s="5"/>
       <c r="F58" t="s">
         <v>59</v>
       </c>
@@ -5135,38 +5189,38 @@
         <f>IF(OR(SUM(G54:G55)=2,AND(SUM(G54:G55)=1,G56=0)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="I58" s="5" t="s">
+      <c r="I58" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="J58" s="5"/>
-      <c r="K58" s="5"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
       <c r="L58">
         <f>IF(ISEVEN(SUM(Q56:Y56)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="N58" s="5" t="s">
+      <c r="N58" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="O58" s="5"/>
-      <c r="P58" s="5"/>
+      <c r="O58" s="8"/>
+      <c r="P58" s="8"/>
       <c r="Q58">
         <f>IF(OR(SUM(V54:V55)=2,AND(SUM(V54:V55)=1,V56=0)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="S58" s="5" t="s">
+      <c r="S58" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="T58" s="5"/>
-      <c r="U58" s="5"/>
+      <c r="T58" s="8"/>
+      <c r="U58" s="8"/>
       <c r="V58">
         <f>IF(SUM(G56:Y56)=0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="X58" s="5" t="s">
+      <c r="X58" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="Y58" s="5"/>
-      <c r="Z58" s="5"/>
+      <c r="Y58" s="8"/>
+      <c r="Z58" s="8"/>
       <c r="AA58">
         <f>G56</f>
         <v>0</v>
@@ -5178,22 +5232,47 @@
         <f>IF(OR(SUM(G54:G55)=2,AND(SUM(G54:G55)=1,G56=0)), 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="AG58" s="6"/>
-      <c r="AH58" s="6"/>
-      <c r="AI58" s="6"/>
-      <c r="AJ58" s="6"/>
-      <c r="AK58" s="6"/>
+      <c r="AG58" s="7"/>
+      <c r="AH58" s="7"/>
+      <c r="AI58" s="7"/>
+      <c r="AJ58" s="7"/>
+      <c r="AK58" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="C54:C58"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="AC54:AC55"/>
-    <mergeCell ref="AG54:AK58"/>
-    <mergeCell ref="I58:K58"/>
-    <mergeCell ref="N58:P58"/>
-    <mergeCell ref="S58:U58"/>
-    <mergeCell ref="X58:Z58"/>
+    <mergeCell ref="AG18:AK22"/>
+    <mergeCell ref="AG24:AK28"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="AC18:AC19"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="S22:U22"/>
+    <mergeCell ref="X22:Z22"/>
+    <mergeCell ref="AC24:AC25"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="S28:U28"/>
+    <mergeCell ref="X28:Z28"/>
+    <mergeCell ref="AC30:AC31"/>
+    <mergeCell ref="AG30:AK34"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="N34:P34"/>
+    <mergeCell ref="S34:U34"/>
+    <mergeCell ref="X34:Z34"/>
+    <mergeCell ref="AC36:AC37"/>
+    <mergeCell ref="AG36:AK40"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="N40:P40"/>
+    <mergeCell ref="S40:U40"/>
+    <mergeCell ref="X40:Z40"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="C36:C40"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E24:E25"/>
     <mergeCell ref="G2:Y2"/>
     <mergeCell ref="C48:C52"/>
     <mergeCell ref="E48:E49"/>
@@ -5210,46 +5289,21 @@
     <mergeCell ref="S46:U46"/>
     <mergeCell ref="X46:Z46"/>
     <mergeCell ref="C18:C22"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="C36:C40"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="AC36:AC37"/>
-    <mergeCell ref="AG36:AK40"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="N40:P40"/>
-    <mergeCell ref="S40:U40"/>
-    <mergeCell ref="X40:Z40"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="AC30:AC31"/>
-    <mergeCell ref="AG30:AK34"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="N34:P34"/>
-    <mergeCell ref="S34:U34"/>
-    <mergeCell ref="X34:Z34"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="AC24:AC25"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="S28:U28"/>
-    <mergeCell ref="X28:Z28"/>
-    <mergeCell ref="AG18:AK22"/>
-    <mergeCell ref="AG24:AK28"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="AC18:AC19"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="S22:U22"/>
-    <mergeCell ref="X22:Z22"/>
+    <mergeCell ref="C54:C58"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="AC54:AC55"/>
+    <mergeCell ref="AG54:AK58"/>
+    <mergeCell ref="I58:K58"/>
+    <mergeCell ref="N58:P58"/>
+    <mergeCell ref="S58:U58"/>
+    <mergeCell ref="X58:Z58"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G4:Y7">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added conversion from decimal to binary
</commit_message>
<xml_diff>
--- a/Informatics/lab4.xlsx
+++ b/Informatics/lab4.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\ITMO-Labs\Informatics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1553B4D3-CCB8-4AEB-98F0-2DA3E262472F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF55190-5460-488B-9EA0-130B960FAF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B976E2FC-2D12-4AD0-A34B-F86A3C86067F}"/>
   </bookViews>
@@ -342,7 +342,18 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1683,10 +1694,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA87596-DBE3-4633-8D29-CBA19FAAD7C8}">
+  <sheetPr codeName="Лист1"/>
   <dimension ref="A1:AK58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1755,60 +1767,76 @@
         <v>31</v>
       </c>
       <c r="G4">
+        <f>IF($C4 - 2 ^ 15 &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="H4">
+        <f>IF($C4 - 2 ^ 14 - ($G4 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="I4">
+        <f>IF($C4 - 2 ^ 13 - ($H4 * 2 ^ 14) - ($G4 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="J4">
+        <f>IF($C4 - 2 ^ 12 - ($I4 * 2 ^ 13) - ($H4 * 2 ^ 14) - ($G4 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>55</v>
       </c>
       <c r="L4">
+        <f>IF($C4 - 2 ^ 11 - ($J4 * 2 ^ 12) - ($I4 * 2 ^ 13) - ($H4 * 2 ^ 14) - ($G4 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="M4">
+        <f>IF($C4 - 2 ^ 10 - ($L4 * 2 ^ 11) - ($J4 * 2 ^ 12) - ($I4 * 2 ^ 13) - ($H4 * 2 ^ 14) - ($G4 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="N4">
+        <f>IF($C4 - 2 ^ 9 - ($M4 * 2 ^ 10) - ($L4 * 2 ^ 11) - ($J4 * 2 ^ 12) - ($I4 * 2 ^ 13) - ($H4 * 2 ^ 14) - ($G4 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="O4">
+        <f>IF($C4 - 2 ^ 8 - ($N4 * 2 ^ 9) - ($M4 * 2 ^ 10) - ($L4 * 2 ^ 11) - ($J4 * 2 ^ 12) - ($I4 * 2 ^ 13) - ($H4 * 2 ^ 14) - ($G4 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>55</v>
       </c>
       <c r="Q4">
+        <f>IF($C4 - 2 ^ 7 - ($O4 * 2 ^ 8) - ($N4 * 2 ^ 9) - ($M4 * 2 ^ 10) - ($L4 * 2 ^ 11) - ($J4 * 2 ^ 12) - ($I4 * 2 ^ 13) - ($H4 * 2 ^ 14) - ($G4 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="R4">
+        <f>IF($C4 - 2 ^ 6 - ($Q4 * 2 ^ 7) - ($O4 * 2 ^ 8) - ($N4 * 2 ^ 9) - ($M4 * 2 ^ 10) - ($L4 * 2 ^ 11) - ($J4 * 2 ^ 12) - ($I4 * 2 ^ 13) - ($H4 * 2 ^ 14) - ($G4 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="S4">
+        <f>IF($C4 - 2 ^ 5 - ($R4 * 2 ^ 6) - ($Q4 * 2 ^ 7) - ($O4 * 2 ^ 8) - ($N4 * 2 ^ 9) - ($M4 * 2 ^ 10) - ($L4 * 2 ^ 11) - ($J4 * 2 ^ 12) - ($I4 * 2 ^ 13) - ($H4 * 2 ^ 14) - ($G4 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="T4">
+        <f>IF($C4 - 2 ^ 4 - ($S4 * 2 ^ 5) - ($R4 * 2 ^ 6) - ($Q4 * 2 ^ 7) - ($O4 * 2 ^ 8) - ($N4 * 2 ^ 9) - ($M4 * 2 ^ 10) - ($L4 * 2 ^ 11) - ($J4 * 2 ^ 12) - ($I4 * 2 ^ 13) - ($H4 * 2 ^ 14) - ($G4 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="U4" s="2" t="s">
         <v>55</v>
       </c>
       <c r="V4">
+        <f>IF($C4 - 2 ^ 3 - ($T4 * 2 ^ 4) - ($S4 * 2 ^ 5) - ($R4 * 2 ^ 6) - ($Q4 * 2 ^ 7) - ($O4 * 2 ^ 8) - ($N4 * 2 ^ 9) - ($M4 * 2 ^ 10) - ($L4 * 2 ^ 11) - ($J4 * 2 ^ 12) - ($I4 * 2 ^ 13) - ($H4 * 2 ^ 14) - ($G4 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="W4">
+        <f>IF($C4 - 2 ^ 2 - ($V4 * 2 ^ 3) - ($T4 * 2 ^ 4) - ($S4 * 2 ^ 5) - ($R4 * 2 ^ 6) - ($Q4 * 2 ^ 7) - ($O4 * 2 ^ 8) - ($N4 * 2 ^ 9) - ($M4 * 2 ^ 10) - ($L4 * 2 ^ 11) - ($J4 * 2 ^ 12) - ($I4 * 2 ^ 13) - ($H4 * 2 ^ 14) - ($G4 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="X4">
+        <f>IF($C4 - 2 - ($W4 * 2 ^ 2) - ($V4 * 2 ^ 3) - ($T4 * 2 ^ 4) - ($S4 * 2 ^ 5) - ($R4 * 2 ^ 6) - ($Q4 * 2 ^ 7) - ($O4 * 2 ^ 8) - ($N4 * 2 ^ 9) - ($M4 * 2 ^ 10) - ($L4 * 2 ^ 11) - ($J4 * 2 ^ 12) - ($I4 * 2 ^ 13) - ($H4 * 2 ^ 14) - ($G4 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="Y4">
+        <f>IF($C4 - 1 - ($X4 * 2) - ($W4 * 2 ^ 2) - ($V4 * 2 ^ 3) - ($T4 * 2 ^ 4) - ($S4 * 2 ^ 5) - ($R4 * 2 ^ 6) - ($Q4 * 2 ^ 7) - ($O4 * 2 ^ 8) - ($N4 * 2 ^ 9) - ($M4 * 2 ^ 10) - ($L4 * 2 ^ 11) - ($J4 * 2 ^ 12) - ($I4 * 2 ^ 13) - ($H4 * 2 ^ 14) - ($G4 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1827,60 +1855,76 @@
         <v>38</v>
       </c>
       <c r="G5">
+        <f>IF($C5 - 2 ^ 15 &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="H5">
+        <f>IF($C5 - 2 ^ 14 - ($G5 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="I5">
+        <f>IF($C5 - 2 ^ 13 - ($H5 * 2 ^ 14) - ($G5 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="J5">
+        <f>IF($C5 - 2 ^ 12 - ($I5 * 2 ^ 13) - ($H5 * 2 ^ 14) - ($G5 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>55</v>
       </c>
       <c r="L5">
+        <f>IF($C5 - 2 ^ 11 - ($J5 * 2 ^ 12) - ($I5 * 2 ^ 13) - ($H5 * 2 ^ 14) - ($G5 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="M5">
+        <f>IF($C5 - 2 ^ 10 - ($L5 * 2 ^ 11) - ($J5 * 2 ^ 12) - ($I5 * 2 ^ 13) - ($H5 * 2 ^ 14) - ($G5 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="N5">
+        <f>IF($C5 - 2 ^ 9 - ($M5 * 2 ^ 10) - ($L5 * 2 ^ 11) - ($J5 * 2 ^ 12) - ($I5 * 2 ^ 13) - ($H5 * 2 ^ 14) - ($G5 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="O5">
+        <f>IF($C5 - 2 ^ 8 - ($N5 * 2 ^ 9) - ($M5 * 2 ^ 10) - ($L5 * 2 ^ 11) - ($J5 * 2 ^ 12) - ($I5 * 2 ^ 13) - ($H5 * 2 ^ 14) - ($G5 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="P5" s="2" t="s">
         <v>55</v>
       </c>
       <c r="Q5">
+        <f>IF($C5 - 2 ^ 7 - ($O5 * 2 ^ 8) - ($N5 * 2 ^ 9) - ($M5 * 2 ^ 10) - ($L5 * 2 ^ 11) - ($J5 * 2 ^ 12) - ($I5 * 2 ^ 13) - ($H5 * 2 ^ 14) - ($G5 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="R5">
+        <f>IF($C5 - 2 ^ 6 - ($Q5 * 2 ^ 7) - ($O5 * 2 ^ 8) - ($N5 * 2 ^ 9) - ($M5 * 2 ^ 10) - ($L5 * 2 ^ 11) - ($J5 * 2 ^ 12) - ($I5 * 2 ^ 13) - ($H5 * 2 ^ 14) - ($G5 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="S5">
+        <f>IF($C5 - 2 ^ 5 - ($R5 * 2 ^ 6) - ($Q5 * 2 ^ 7) - ($O5 * 2 ^ 8) - ($N5 * 2 ^ 9) - ($M5 * 2 ^ 10) - ($L5 * 2 ^ 11) - ($J5 * 2 ^ 12) - ($I5 * 2 ^ 13) - ($H5 * 2 ^ 14) - ($G5 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="T5">
+        <f>IF($C5 - 2 ^ 4 - ($S5 * 2 ^ 5) - ($R5 * 2 ^ 6) - ($Q5 * 2 ^ 7) - ($O5 * 2 ^ 8) - ($N5 * 2 ^ 9) - ($M5 * 2 ^ 10) - ($L5 * 2 ^ 11) - ($J5 * 2 ^ 12) - ($I5 * 2 ^ 13) - ($H5 * 2 ^ 14) - ($G5 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="U5" s="2" t="s">
         <v>55</v>
       </c>
       <c r="V5">
+        <f>IF($C5 - 2 ^ 3 - ($T5 * 2 ^ 4) - ($S5 * 2 ^ 5) - ($R5 * 2 ^ 6) - ($Q5 * 2 ^ 7) - ($O5 * 2 ^ 8) - ($N5 * 2 ^ 9) - ($M5 * 2 ^ 10) - ($L5 * 2 ^ 11) - ($J5 * 2 ^ 12) - ($I5 * 2 ^ 13) - ($H5 * 2 ^ 14) - ($G5 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="W5">
+        <f>IF($C5 - 2 ^ 2 - ($V5 * 2 ^ 3) - ($T5 * 2 ^ 4) - ($S5 * 2 ^ 5) - ($R5 * 2 ^ 6) - ($Q5 * 2 ^ 7) - ($O5 * 2 ^ 8) - ($N5 * 2 ^ 9) - ($M5 * 2 ^ 10) - ($L5 * 2 ^ 11) - ($J5 * 2 ^ 12) - ($I5 * 2 ^ 13) - ($H5 * 2 ^ 14) - ($G5 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="X5">
+        <f>IF($C5 - 2 - ($W5 * 2 ^ 2) - ($V5 * 2 ^ 3) - ($T5 * 2 ^ 4) - ($S5 * 2 ^ 5) - ($R5 * 2 ^ 6) - ($Q5 * 2 ^ 7) - ($O5 * 2 ^ 8) - ($N5 * 2 ^ 9) - ($M5 * 2 ^ 10) - ($L5 * 2 ^ 11) - ($J5 * 2 ^ 12) - ($I5 * 2 ^ 13) - ($H5 * 2 ^ 14) - ($G5 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="Y5">
+        <f>IF($C5 - 1 - ($X5 * 2) - ($W5 * 2 ^ 2) - ($V5 * 2 ^ 3) - ($T5 * 2 ^ 4) - ($S5 * 2 ^ 5) - ($R5 * 2 ^ 6) - ($Q5 * 2 ^ 7) - ($O5 * 2 ^ 8) - ($N5 * 2 ^ 9) - ($M5 * 2 ^ 10) - ($L5 * 2 ^ 11) - ($J5 * 2 ^ 12) - ($I5 * 2 ^ 13) - ($H5 * 2 ^ 14) - ($G5 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
     </row>
@@ -1899,60 +1943,76 @@
         <v>39</v>
       </c>
       <c r="G6">
+        <f>IF($C6 - 2 ^ 15 &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="H6">
+        <f>IF($C6 - 2 ^ 14 - ($G6 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="I6">
+        <f>IF($C6 - 2 ^ 13 - ($H6 * 2 ^ 14) - ($G6 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="J6">
+        <f>IF($C6 - 2 ^ 12 - ($I6 * 2 ^ 13) - ($H6 * 2 ^ 14) - ($G6 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>55</v>
       </c>
       <c r="L6">
+        <f>IF($C6 - 2 ^ 11 - ($J6 * 2 ^ 12) - ($I6 * 2 ^ 13) - ($H6 * 2 ^ 14) - ($G6 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="M6">
+        <f>IF($C6 - 2 ^ 10 - ($L6 * 2 ^ 11) - ($J6 * 2 ^ 12) - ($I6 * 2 ^ 13) - ($H6 * 2 ^ 14) - ($G6 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="N6">
+        <f>IF($C6 - 2 ^ 9 - ($M6 * 2 ^ 10) - ($L6 * 2 ^ 11) - ($J6 * 2 ^ 12) - ($I6 * 2 ^ 13) - ($H6 * 2 ^ 14) - ($G6 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="O6">
+        <f>IF($C6 - 2 ^ 8 - ($N6 * 2 ^ 9) - ($M6 * 2 ^ 10) - ($L6 * 2 ^ 11) - ($J6 * 2 ^ 12) - ($I6 * 2 ^ 13) - ($H6 * 2 ^ 14) - ($G6 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>55</v>
       </c>
       <c r="Q6">
+        <f>IF($C6 - 2 ^ 7 - ($O6 * 2 ^ 8) - ($N6 * 2 ^ 9) - ($M6 * 2 ^ 10) - ($L6 * 2 ^ 11) - ($J6 * 2 ^ 12) - ($I6 * 2 ^ 13) - ($H6 * 2 ^ 14) - ($G6 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="R6">
+        <f>IF($C6 - 2 ^ 6 - ($Q6 * 2 ^ 7) - ($O6 * 2 ^ 8) - ($N6 * 2 ^ 9) - ($M6 * 2 ^ 10) - ($L6 * 2 ^ 11) - ($J6 * 2 ^ 12) - ($I6 * 2 ^ 13) - ($H6 * 2 ^ 14) - ($G6 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="S6">
+        <f>IF($C6 - 2 ^ 5 - ($R6 * 2 ^ 6) - ($Q6 * 2 ^ 7) - ($O6 * 2 ^ 8) - ($N6 * 2 ^ 9) - ($M6 * 2 ^ 10) - ($L6 * 2 ^ 11) - ($J6 * 2 ^ 12) - ($I6 * 2 ^ 13) - ($H6 * 2 ^ 14) - ($G6 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="T6">
+        <f>IF($C6 - 2 ^ 4 - ($S6 * 2 ^ 5) - ($R6 * 2 ^ 6) - ($Q6 * 2 ^ 7) - ($O6 * 2 ^ 8) - ($N6 * 2 ^ 9) - ($M6 * 2 ^ 10) - ($L6 * 2 ^ 11) - ($J6 * 2 ^ 12) - ($I6 * 2 ^ 13) - ($H6 * 2 ^ 14) - ($G6 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="U6" s="2" t="s">
         <v>55</v>
       </c>
       <c r="V6">
+        <f>IF($C6 - 2 ^ 3 - ($T6 * 2 ^ 4) - ($S6 * 2 ^ 5) - ($R6 * 2 ^ 6) - ($Q6 * 2 ^ 7) - ($O6 * 2 ^ 8) - ($N6 * 2 ^ 9) - ($M6 * 2 ^ 10) - ($L6 * 2 ^ 11) - ($J6 * 2 ^ 12) - ($I6 * 2 ^ 13) - ($H6 * 2 ^ 14) - ($G6 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="W6">
+        <f>IF($C6 - 2 ^ 2 - ($V6 * 2 ^ 3) - ($T6 * 2 ^ 4) - ($S6 * 2 ^ 5) - ($R6 * 2 ^ 6) - ($Q6 * 2 ^ 7) - ($O6 * 2 ^ 8) - ($N6 * 2 ^ 9) - ($M6 * 2 ^ 10) - ($L6 * 2 ^ 11) - ($J6 * 2 ^ 12) - ($I6 * 2 ^ 13) - ($H6 * 2 ^ 14) - ($G6 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="X6">
+        <f>IF($C6 - 2 - ($W6 * 2 ^ 2) - ($V6 * 2 ^ 3) - ($T6 * 2 ^ 4) - ($S6 * 2 ^ 5) - ($R6 * 2 ^ 6) - ($Q6 * 2 ^ 7) - ($O6 * 2 ^ 8) - ($N6 * 2 ^ 9) - ($M6 * 2 ^ 10) - ($L6 * 2 ^ 11) - ($J6 * 2 ^ 12) - ($I6 * 2 ^ 13) - ($H6 * 2 ^ 14) - ($G6 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="Y6">
+        <f>IF($C6 - 1 - ($X6 * 2) - ($W6 * 2 ^ 2) - ($V6 * 2 ^ 3) - ($T6 * 2 ^ 4) - ($S6 * 2 ^ 5) - ($R6 * 2 ^ 6) - ($Q6 * 2 ^ 7) - ($O6 * 2 ^ 8) - ($N6 * 2 ^ 9) - ($M6 * 2 ^ 10) - ($L6 * 2 ^ 11) - ($J6 * 2 ^ 12) - ($I6 * 2 ^ 13) - ($H6 * 2 ^ 14) - ($G6 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
     </row>
@@ -1971,60 +2031,76 @@
         <v>40</v>
       </c>
       <c r="G7">
+        <f>IF($C7 - 2 ^ 15 &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="H7">
+        <f>IF($C7 - 2 ^ 14 - ($G7 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="I7">
+        <f>IF($C7 - 2 ^ 13 - ($H7 * 2 ^ 14) - ($G7 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="J7">
+        <f>IF($C7 - 2 ^ 12 - ($I7 * 2 ^ 13) - ($H7 * 2 ^ 14) - ($G7 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>55</v>
       </c>
       <c r="L7">
+        <f>IF($C7 - 2 ^ 11 - ($J7 * 2 ^ 12) - ($I7 * 2 ^ 13) - ($H7 * 2 ^ 14) - ($G7 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="M7">
+        <f>IF($C7 - 2 ^ 10 - ($L7 * 2 ^ 11) - ($J7 * 2 ^ 12) - ($I7 * 2 ^ 13) - ($H7 * 2 ^ 14) - ($G7 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="N7">
+        <f>IF($C7 - 2 ^ 9 - ($M7 * 2 ^ 10) - ($L7 * 2 ^ 11) - ($J7 * 2 ^ 12) - ($I7 * 2 ^ 13) - ($H7 * 2 ^ 14) - ($G7 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="O7">
+        <f>IF($C7 - 2 ^ 8 - ($N7 * 2 ^ 9) - ($M7 * 2 ^ 10) - ($L7 * 2 ^ 11) - ($J7 * 2 ^ 12) - ($I7 * 2 ^ 13) - ($H7 * 2 ^ 14) - ($G7 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>55</v>
       </c>
       <c r="Q7">
+        <f>IF($C7 - 2 ^ 7 - ($O7 * 2 ^ 8) - ($N7 * 2 ^ 9) - ($M7 * 2 ^ 10) - ($L7 * 2 ^ 11) - ($J7 * 2 ^ 12) - ($I7 * 2 ^ 13) - ($H7 * 2 ^ 14) - ($G7 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="R7">
+        <f>IF($C7 - 2 ^ 6 - ($Q7 * 2 ^ 7) - ($O7 * 2 ^ 8) - ($N7 * 2 ^ 9) - ($M7 * 2 ^ 10) - ($L7 * 2 ^ 11) - ($J7 * 2 ^ 12) - ($I7 * 2 ^ 13) - ($H7 * 2 ^ 14) - ($G7 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="S7">
+        <f>IF($C7 - 2 ^ 5 - ($R7 * 2 ^ 6) - ($Q7 * 2 ^ 7) - ($O7 * 2 ^ 8) - ($N7 * 2 ^ 9) - ($M7 * 2 ^ 10) - ($L7 * 2 ^ 11) - ($J7 * 2 ^ 12) - ($I7 * 2 ^ 13) - ($H7 * 2 ^ 14) - ($G7 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="T7">
+        <f>IF($C7 - 2 ^ 4 - ($S7 * 2 ^ 5) - ($R7 * 2 ^ 6) - ($Q7 * 2 ^ 7) - ($O7 * 2 ^ 8) - ($N7 * 2 ^ 9) - ($M7 * 2 ^ 10) - ($L7 * 2 ^ 11) - ($J7 * 2 ^ 12) - ($I7 * 2 ^ 13) - ($H7 * 2 ^ 14) - ($G7 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="U7" s="2" t="s">
         <v>55</v>
       </c>
       <c r="V7">
+        <f>IF($C7 - 2 ^ 3 - ($T7 * 2 ^ 4) - ($S7 * 2 ^ 5) - ($R7 * 2 ^ 6) - ($Q7 * 2 ^ 7) - ($O7 * 2 ^ 8) - ($N7 * 2 ^ 9) - ($M7 * 2 ^ 10) - ($L7 * 2 ^ 11) - ($J7 * 2 ^ 12) - ($I7 * 2 ^ 13) - ($H7 * 2 ^ 14) - ($G7 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="W7">
+        <f>IF($C7 - 2 ^ 2 - ($V7 * 2 ^ 3) - ($T7 * 2 ^ 4) - ($S7 * 2 ^ 5) - ($R7 * 2 ^ 6) - ($Q7 * 2 ^ 7) - ($O7 * 2 ^ 8) - ($N7 * 2 ^ 9) - ($M7 * 2 ^ 10) - ($L7 * 2 ^ 11) - ($J7 * 2 ^ 12) - ($I7 * 2 ^ 13) - ($H7 * 2 ^ 14) - ($G7 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="X7">
+        <f>IF($C7 - 2 - ($W7 * 2 ^ 2) - ($V7 * 2 ^ 3) - ($T7 * 2 ^ 4) - ($S7 * 2 ^ 5) - ($R7 * 2 ^ 6) - ($Q7 * 2 ^ 7) - ($O7 * 2 ^ 8) - ($N7 * 2 ^ 9) - ($M7 * 2 ^ 10) - ($L7 * 2 ^ 11) - ($J7 * 2 ^ 12) - ($I7 * 2 ^ 13) - ($H7 * 2 ^ 14) - ($G7 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="Y7">
+        <f>IF($C7 - 1 - ($X7 * 2) - ($W7 * 2 ^ 2) - ($V7 * 2 ^ 3) - ($T7 * 2 ^ 4) - ($S7 * 2 ^ 5) - ($R7 * 2 ^ 6) - ($Q7 * 2 ^ 7) - ($O7 * 2 ^ 8) - ($N7 * 2 ^ 9) - ($M7 * 2 ^ 10) - ($L7 * 2 ^ 11) - ($J7 * 2 ^ 12) - ($I7 * 2 ^ 13) - ($H7 * 2 ^ 14) - ($G7 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -2043,60 +2119,76 @@
         <v>41</v>
       </c>
       <c r="G8">
+        <f>IF($C8 - 2 ^ 15 &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="H8">
+        <f>IF($C8 - 2 ^ 14 - ($G8 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="I8">
+        <f>IF($C8 - 2 ^ 13 - ($H8 * 2 ^ 14) - ($G8 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="J8">
+        <f>IF($C8 - 2 ^ 12 - ($I8 * 2 ^ 13) - ($H8 * 2 ^ 14) - ($G8 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>55</v>
       </c>
       <c r="L8">
+        <f>IF($C8 - 2 ^ 11 - ($J8 * 2 ^ 12) - ($I8 * 2 ^ 13) - ($H8 * 2 ^ 14) - ($G8 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="M8">
+        <f>IF($C8 - 2 ^ 10 - ($L8 * 2 ^ 11) - ($J8 * 2 ^ 12) - ($I8 * 2 ^ 13) - ($H8 * 2 ^ 14) - ($G8 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="N8">
+        <f>IF($C8 - 2 ^ 9 - ($M8 * 2 ^ 10) - ($L8 * 2 ^ 11) - ($J8 * 2 ^ 12) - ($I8 * 2 ^ 13) - ($H8 * 2 ^ 14) - ($G8 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="O8">
+        <f>IF($C8 - 2 ^ 8 - ($N8 * 2 ^ 9) - ($M8 * 2 ^ 10) - ($L8 * 2 ^ 11) - ($J8 * 2 ^ 12) - ($I8 * 2 ^ 13) - ($H8 * 2 ^ 14) - ($G8 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="P8" s="2" t="s">
         <v>55</v>
       </c>
       <c r="Q8">
+        <f>IF($C8 - 2 ^ 7 - ($O8 * 2 ^ 8) - ($N8 * 2 ^ 9) - ($M8 * 2 ^ 10) - ($L8 * 2 ^ 11) - ($J8 * 2 ^ 12) - ($I8 * 2 ^ 13) - ($H8 * 2 ^ 14) - ($G8 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="R8">
+        <f>IF($C8 - 2 ^ 6 - ($Q8 * 2 ^ 7) - ($O8 * 2 ^ 8) - ($N8 * 2 ^ 9) - ($M8 * 2 ^ 10) - ($L8 * 2 ^ 11) - ($J8 * 2 ^ 12) - ($I8 * 2 ^ 13) - ($H8 * 2 ^ 14) - ($G8 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="S8">
+        <f>IF($C8 - 2 ^ 5 - ($R8 * 2 ^ 6) - ($Q8 * 2 ^ 7) - ($O8 * 2 ^ 8) - ($N8 * 2 ^ 9) - ($M8 * 2 ^ 10) - ($L8 * 2 ^ 11) - ($J8 * 2 ^ 12) - ($I8 * 2 ^ 13) - ($H8 * 2 ^ 14) - ($G8 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="T8">
+        <f>IF($C8 - 2 ^ 4 - ($S8 * 2 ^ 5) - ($R8 * 2 ^ 6) - ($Q8 * 2 ^ 7) - ($O8 * 2 ^ 8) - ($N8 * 2 ^ 9) - ($M8 * 2 ^ 10) - ($L8 * 2 ^ 11) - ($J8 * 2 ^ 12) - ($I8 * 2 ^ 13) - ($H8 * 2 ^ 14) - ($G8 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="U8" s="2" t="s">
         <v>55</v>
       </c>
       <c r="V8">
+        <f>IF($C8 - 2 ^ 3 - ($T8 * 2 ^ 4) - ($S8 * 2 ^ 5) - ($R8 * 2 ^ 6) - ($Q8 * 2 ^ 7) - ($O8 * 2 ^ 8) - ($N8 * 2 ^ 9) - ($M8 * 2 ^ 10) - ($L8 * 2 ^ 11) - ($J8 * 2 ^ 12) - ($I8 * 2 ^ 13) - ($H8 * 2 ^ 14) - ($G8 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="W8">
+        <f>IF($C8 - 2 ^ 2 - ($V8 * 2 ^ 3) - ($T8 * 2 ^ 4) - ($S8 * 2 ^ 5) - ($R8 * 2 ^ 6) - ($Q8 * 2 ^ 7) - ($O8 * 2 ^ 8) - ($N8 * 2 ^ 9) - ($M8 * 2 ^ 10) - ($L8 * 2 ^ 11) - ($J8 * 2 ^ 12) - ($I8 * 2 ^ 13) - ($H8 * 2 ^ 14) - ($G8 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="X8">
+        <f>IF($C8 - 2 - ($W8 * 2 ^ 2) - ($V8 * 2 ^ 3) - ($T8 * 2 ^ 4) - ($S8 * 2 ^ 5) - ($R8 * 2 ^ 6) - ($Q8 * 2 ^ 7) - ($O8 * 2 ^ 8) - ($N8 * 2 ^ 9) - ($M8 * 2 ^ 10) - ($L8 * 2 ^ 11) - ($J8 * 2 ^ 12) - ($I8 * 2 ^ 13) - ($H8 * 2 ^ 14) - ($G8 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="Y8">
+        <f>IF($C8 - 1 - ($X8 * 2) - ($W8 * 2 ^ 2) - ($V8 * 2 ^ 3) - ($T8 * 2 ^ 4) - ($S8 * 2 ^ 5) - ($R8 * 2 ^ 6) - ($Q8 * 2 ^ 7) - ($O8 * 2 ^ 8) - ($N8 * 2 ^ 9) - ($M8 * 2 ^ 10) - ($L8 * 2 ^ 11) - ($J8 * 2 ^ 12) - ($I8 * 2 ^ 13) - ($H8 * 2 ^ 14) - ($G8 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2115,60 +2207,76 @@
         <v>42</v>
       </c>
       <c r="G9">
+        <f>IF($C9 - 2 ^ 15 &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="H9">
+        <f>IF($C9 - 2 ^ 14 - ($G9 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="I9">
+        <f>IF($C9 - 2 ^ 13 - ($H9 * 2 ^ 14) - ($G9 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="J9">
+        <f>IF($C9 - 2 ^ 12 - ($I9 * 2 ^ 13) - ($H9 * 2 ^ 14) - ($G9 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>55</v>
       </c>
       <c r="L9">
+        <f>IF($C9 - 2 ^ 11 - ($J9 * 2 ^ 12) - ($I9 * 2 ^ 13) - ($H9 * 2 ^ 14) - ($G9 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="M9">
+        <f>IF($C9 - 2 ^ 10 - ($L9 * 2 ^ 11) - ($J9 * 2 ^ 12) - ($I9 * 2 ^ 13) - ($H9 * 2 ^ 14) - ($G9 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="N9">
+        <f>IF($C9 - 2 ^ 9 - ($M9 * 2 ^ 10) - ($L9 * 2 ^ 11) - ($J9 * 2 ^ 12) - ($I9 * 2 ^ 13) - ($H9 * 2 ^ 14) - ($G9 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="O9">
+        <f>IF($C9 - 2 ^ 8 - ($N9 * 2 ^ 9) - ($M9 * 2 ^ 10) - ($L9 * 2 ^ 11) - ($J9 * 2 ^ 12) - ($I9 * 2 ^ 13) - ($H9 * 2 ^ 14) - ($G9 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>55</v>
       </c>
       <c r="Q9">
+        <f>IF($C9 - 2 ^ 7 - ($O9 * 2 ^ 8) - ($N9 * 2 ^ 9) - ($M9 * 2 ^ 10) - ($L9 * 2 ^ 11) - ($J9 * 2 ^ 12) - ($I9 * 2 ^ 13) - ($H9 * 2 ^ 14) - ($G9 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="R9">
+        <f>IF($C9 - 2 ^ 6 - ($Q9 * 2 ^ 7) - ($O9 * 2 ^ 8) - ($N9 * 2 ^ 9) - ($M9 * 2 ^ 10) - ($L9 * 2 ^ 11) - ($J9 * 2 ^ 12) - ($I9 * 2 ^ 13) - ($H9 * 2 ^ 14) - ($G9 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="S9">
+        <f>IF($C9 - 2 ^ 5 - ($R9 * 2 ^ 6) - ($Q9 * 2 ^ 7) - ($O9 * 2 ^ 8) - ($N9 * 2 ^ 9) - ($M9 * 2 ^ 10) - ($L9 * 2 ^ 11) - ($J9 * 2 ^ 12) - ($I9 * 2 ^ 13) - ($H9 * 2 ^ 14) - ($G9 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="T9">
+        <f>IF($C9 - 2 ^ 4 - ($S9 * 2 ^ 5) - ($R9 * 2 ^ 6) - ($Q9 * 2 ^ 7) - ($O9 * 2 ^ 8) - ($N9 * 2 ^ 9) - ($M9 * 2 ^ 10) - ($L9 * 2 ^ 11) - ($J9 * 2 ^ 12) - ($I9 * 2 ^ 13) - ($H9 * 2 ^ 14) - ($G9 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="U9" s="2" t="s">
         <v>55</v>
       </c>
       <c r="V9">
+        <f>IF($C9 - 2 ^ 3 - ($T9 * 2 ^ 4) - ($S9 * 2 ^ 5) - ($R9 * 2 ^ 6) - ($Q9 * 2 ^ 7) - ($O9 * 2 ^ 8) - ($N9 * 2 ^ 9) - ($M9 * 2 ^ 10) - ($L9 * 2 ^ 11) - ($J9 * 2 ^ 12) - ($I9 * 2 ^ 13) - ($H9 * 2 ^ 14) - ($G9 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="W9">
+        <f>IF($C9 - 2 ^ 2 - ($V9 * 2 ^ 3) - ($T9 * 2 ^ 4) - ($S9 * 2 ^ 5) - ($R9 * 2 ^ 6) - ($Q9 * 2 ^ 7) - ($O9 * 2 ^ 8) - ($N9 * 2 ^ 9) - ($M9 * 2 ^ 10) - ($L9 * 2 ^ 11) - ($J9 * 2 ^ 12) - ($I9 * 2 ^ 13) - ($H9 * 2 ^ 14) - ($G9 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="X9">
+        <f>IF($C9 - 2 - ($W9 * 2 ^ 2) - ($V9 * 2 ^ 3) - ($T9 * 2 ^ 4) - ($S9 * 2 ^ 5) - ($R9 * 2 ^ 6) - ($Q9 * 2 ^ 7) - ($O9 * 2 ^ 8) - ($N9 * 2 ^ 9) - ($M9 * 2 ^ 10) - ($L9 * 2 ^ 11) - ($J9 * 2 ^ 12) - ($I9 * 2 ^ 13) - ($H9 * 2 ^ 14) - ($G9 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="Y9">
+        <f>IF($C9 - 1 - ($X9 * 2) - ($W9 * 2 ^ 2) - ($V9 * 2 ^ 3) - ($T9 * 2 ^ 4) - ($S9 * 2 ^ 5) - ($R9 * 2 ^ 6) - ($Q9 * 2 ^ 7) - ($O9 * 2 ^ 8) - ($N9 * 2 ^ 9) - ($M9 * 2 ^ 10) - ($L9 * 2 ^ 11) - ($J9 * 2 ^ 12) - ($I9 * 2 ^ 13) - ($H9 * 2 ^ 14) - ($G9 * 2 ^ 15) &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5300,10 +5408,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G4:Y7">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5318,6 +5426,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635C2B6A-31FF-4DB8-BD65-8116685FF096}">
+  <sheetPr codeName="Лист2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>